<commit_message>
YTD file for metrics updated for September
</commit_message>
<xml_diff>
--- a/Code/Failure_rate/2021/YTD/2021_YTD.xlsx
+++ b/Code/Failure_rate/2021/YTD/2021_YTD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\USAI\Code\Failure_rate\2021\YTD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C757A60B-5B63-4E68-AC18-89B207955ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5107A9-ADAF-4B35-B6A6-A049EDD344D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3870" yWindow="2445" windowWidth="20550" windowHeight="13785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="1275" windowWidth="20550" windowHeight="13785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6811" uniqueCount="2264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7486" uniqueCount="2456">
   <si>
     <t>RMA_ID</t>
   </si>
@@ -6818,6 +6818,584 @@
   </si>
   <si>
     <t>DRIVER REPLACEMENT NANO MTG-2 20W-500mA 120V-277V DIML6F-EL</t>
+  </si>
+  <si>
+    <t>RMA16099</t>
+  </si>
+  <si>
+    <t>SP-335-01-RD-F-M-21</t>
+  </si>
+  <si>
+    <t>BVLED 4"NC UNV ADPT CONVERSION KIT- RND FLANGED/TRIMLESS TO MLWK-BLACK</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>RMA16098</t>
+  </si>
+  <si>
+    <t>MWF12-41H1-35KS-WH-WH-TRM</t>
+  </si>
+  <si>
+    <t>MICRO WALL WASH FLANGE 12 CELL 41W 3500KS WHITE-WHITE-TRIM</t>
+  </si>
+  <si>
+    <t>RMA16097</t>
+  </si>
+  <si>
+    <t>RMA16096</t>
+  </si>
+  <si>
+    <t>RMA16095</t>
+  </si>
+  <si>
+    <t>CBRC12-24C3-30KS-45-S-BL-AR3-UNV-D6A</t>
+  </si>
+  <si>
+    <t>2.2 CYLINDER RD CROSS BAFF 24W CW 3000KS 45° BEAM-SOLITE LENS-BLACK-AR MOUNT 96" 120-277V D6A</t>
+  </si>
+  <si>
+    <t>RMA16094</t>
+  </si>
+  <si>
+    <t>RMA16093</t>
+  </si>
+  <si>
+    <t>RMA16092</t>
+  </si>
+  <si>
+    <t>RMA16091</t>
+  </si>
+  <si>
+    <t>B4RDF-12G1-35KS-90-NCIC-UNV-D6E-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 BASIC RD DL TRMD 12W CLASSIC 35K 80CRI 90° BEAM NCIC HSG 120-277V ELDO 1% LIN DIM</t>
+  </si>
+  <si>
+    <t>B4RDF-S-AC-AC-TRM</t>
+  </si>
+  <si>
+    <t>BEVELED ROUND TRMD DL/ADJ SOLITE LENS CLEAR MATTE ANOD</t>
+  </si>
+  <si>
+    <t>RMA16090</t>
+  </si>
+  <si>
+    <t>RMA16089</t>
+  </si>
+  <si>
+    <t>LEM-275-32-3022KH</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT-BEVELED 2.2 WG2 32W 90CRI 3000-2200K</t>
+  </si>
+  <si>
+    <t>RMA16088</t>
+  </si>
+  <si>
+    <t>RMA16087</t>
+  </si>
+  <si>
+    <t>B4SDF-16G1-30KS-50-NCSM-UNV-D6E-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 BASIC SQ DL TRMD 16W CLASSIC 30K 80CRI 50° BEAM NCSM HSG 120-277V ELDO 1% LIN DIM</t>
+  </si>
+  <si>
+    <t>RMA16086</t>
+  </si>
+  <si>
+    <t>RMA16085</t>
+  </si>
+  <si>
+    <t>RMA16084</t>
+  </si>
+  <si>
+    <t>RMA16083</t>
+  </si>
+  <si>
+    <t>RMA16081</t>
+  </si>
+  <si>
+    <t>MDM04-13H1-30KH-50-BL-TRM</t>
+  </si>
+  <si>
+    <t>MICRO DOWNLIGHT TRIMLESS/MILLWORK 4 CELL 13W 3000KH 50° BLACK TRIM</t>
+  </si>
+  <si>
+    <t>RMA16080</t>
+  </si>
+  <si>
+    <t>RMA16079</t>
+  </si>
+  <si>
+    <t>RMA16078</t>
+  </si>
+  <si>
+    <t>RMA16077</t>
+  </si>
+  <si>
+    <t>RMA16076</t>
+  </si>
+  <si>
+    <t>MDG06-21H1-35KH-50-BL-BL-GL95-TRM</t>
+  </si>
+  <si>
+    <t>MICRO DL FOR WOODWORKS 6 CELL 21W 3500K 90 CRI 50° BLACK-BLACK GL95 TRIM</t>
+  </si>
+  <si>
+    <t>RMA16075</t>
+  </si>
+  <si>
+    <t>MDG08-27H1-30KH-35-BL-BL-GT31-TRM</t>
+  </si>
+  <si>
+    <t>MICRO DL FOR WOODWORKS 8 CELL 27W 3000K 90 CRI 35° BLACK-BLACK GT31 TRIM</t>
+  </si>
+  <si>
+    <t>RMA16074</t>
+  </si>
+  <si>
+    <t>RMA16073</t>
+  </si>
+  <si>
+    <t>RMA16072</t>
+  </si>
+  <si>
+    <t>LEM-198-32-3022KS</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT BEVELED 2.0 WGD/CCD 32W STD CRI 3000-2200KS</t>
+  </si>
+  <si>
+    <t>RMA16070</t>
+  </si>
+  <si>
+    <t>SP-263-0700-4H</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT-MICRO TRMD NC 21-41W 700mA DIML4H-LT</t>
+  </si>
+  <si>
+    <t>RMA16069</t>
+  </si>
+  <si>
+    <t>RMA16068</t>
+  </si>
+  <si>
+    <t>SP-140-1000-6B</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT - BEVELED 2.1 NC/IC/CP 24 WATT 1000mA 120V-277V-DIML6B EL</t>
+  </si>
+  <si>
+    <t>RMA16066</t>
+  </si>
+  <si>
+    <t>1020-B1-F-10</t>
+  </si>
+  <si>
+    <t>BEVELED BASIC ROUND TRIMMED DOWNLIGHT-DIE CAST BEVEL-WHITE-FROSTED LENS</t>
+  </si>
+  <si>
+    <t>1251-B1-10</t>
+  </si>
+  <si>
+    <t>BEVELED BASIC TRIMMED ROUND WALLWASH-DIE CAST BEVEL WHITE</t>
+  </si>
+  <si>
+    <t>RMA16065</t>
+  </si>
+  <si>
+    <t>RMA16064</t>
+  </si>
+  <si>
+    <t>B4RGM-45-SF-WH-TRM</t>
+  </si>
+  <si>
+    <t>BEVELED RD DL MWRK 45° SLOPED SOLITE FROSTED LENS WHITE BEVEL</t>
+  </si>
+  <si>
+    <t>RMA16063</t>
+  </si>
+  <si>
+    <t>RMA16062</t>
+  </si>
+  <si>
+    <t>7875-10</t>
+  </si>
+  <si>
+    <t>SLIVER ROUND ADJ-VERTICAL GROOVE BLACK BAFFLE-WHITE</t>
+  </si>
+  <si>
+    <t>325CCR</t>
+  </si>
+  <si>
+    <t>325 CONV COLLAR RND WHT</t>
+  </si>
+  <si>
+    <t>325NC-120</t>
+  </si>
+  <si>
+    <t>RECESSED SLIDER HOUSING 50W</t>
+  </si>
+  <si>
+    <t>8177-A</t>
+  </si>
+  <si>
+    <t>LOUVER HEX CELL SIZE A</t>
+  </si>
+  <si>
+    <t>RMA16061</t>
+  </si>
+  <si>
+    <t>RMA16060</t>
+  </si>
+  <si>
+    <t>RMA16059</t>
+  </si>
+  <si>
+    <t>LEM-319-00-40KS</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT MINI X 80 CRI 4000K</t>
+  </si>
+  <si>
+    <t>RMA16058</t>
+  </si>
+  <si>
+    <t>RMA16057</t>
+  </si>
+  <si>
+    <t>RMA16056</t>
+  </si>
+  <si>
+    <t>RMA16055</t>
+  </si>
+  <si>
+    <t>RPA-02-41H1-UNV-D8E</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER MICRO-2 FIXTURES MAX-41W H1 700mA 120-277V D8E</t>
+  </si>
+  <si>
+    <t>RMA16054</t>
+  </si>
+  <si>
+    <t>RMA16052</t>
+  </si>
+  <si>
+    <t>RMA16050</t>
+  </si>
+  <si>
+    <t>RMA16049</t>
+  </si>
+  <si>
+    <t>RMA16048</t>
+  </si>
+  <si>
+    <t>RMA16047</t>
+  </si>
+  <si>
+    <t>B3RGM-45-S-WH-TRM</t>
+  </si>
+  <si>
+    <t>BEVELED MINI RD DL MWRK 45° SLOPED SOLITE CLEAR LENS WHITE BEVEL</t>
+  </si>
+  <si>
+    <t>RMA16046</t>
+  </si>
+  <si>
+    <t>RMA16045</t>
+  </si>
+  <si>
+    <t>RMA16044</t>
+  </si>
+  <si>
+    <t>RMA16043</t>
+  </si>
+  <si>
+    <t>LEM-230-16-30KH</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT BEVELED 2.0 DL/WW 16W HI CRI 3000K</t>
+  </si>
+  <si>
+    <t>SP-141-0700-4</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT BEVELED 2.1 NCSM HSG 16 WATT 700mA-120V-277V-DIML4-LU</t>
+  </si>
+  <si>
+    <t>RMA16042</t>
+  </si>
+  <si>
+    <t>RMA16041</t>
+  </si>
+  <si>
+    <t>RMA16040</t>
+  </si>
+  <si>
+    <t>SP-335-03-RD-F-L</t>
+  </si>
+  <si>
+    <t>BVLED 4”FTA UNV ADPT CONVERSION KIT- RND FLANGED TO TRIMLESS</t>
+  </si>
+  <si>
+    <t>RMA16039</t>
+  </si>
+  <si>
+    <t>RMA16038</t>
+  </si>
+  <si>
+    <t>SP-238-1050</t>
+  </si>
+  <si>
+    <t>REMOTE ELDOLED 600W 0-10V POWER SUPPLY 1050mA</t>
+  </si>
+  <si>
+    <t>RMA16037</t>
+  </si>
+  <si>
+    <t>RMA16036</t>
+  </si>
+  <si>
+    <t>RMA16035</t>
+  </si>
+  <si>
+    <t>B4SDF-32FC1-70-NCSM-UNV-D23X1-WR-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 SQ DL TRMD 32W INFINITE COLOR+ 70°BEAM NCSM HSG 120-277V ELDO DMX 0.1% 8 BIT WIRE SPLICE</t>
+  </si>
+  <si>
+    <t>RMA16034</t>
+  </si>
+  <si>
+    <t>RMA16033</t>
+  </si>
+  <si>
+    <t>P2-110C</t>
+  </si>
+  <si>
+    <t>BEVELED 3" DL CONCENTRIC RING</t>
+  </si>
+  <si>
+    <t>RMA16032</t>
+  </si>
+  <si>
+    <t>LEM-204-00-3022KS</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT BEVELED WGD ADJ 30DEG 18W STD CRI 3000-2200K</t>
+  </si>
+  <si>
+    <t>RMA16031</t>
+  </si>
+  <si>
+    <t>Z3RDL-C-S-WH-TRM</t>
+  </si>
+  <si>
+    <t>TRUE ZERO MINI ROUND DL/ADJ TRMLESS CONCEAL SOLITE LENS WHITE</t>
+  </si>
+  <si>
+    <t>RMA16030</t>
+  </si>
+  <si>
+    <t>RMA16029</t>
+  </si>
+  <si>
+    <t>RMA16028</t>
+  </si>
+  <si>
+    <t>RMA16027</t>
+  </si>
+  <si>
+    <t>RMA16026</t>
+  </si>
+  <si>
+    <t>RMA16025</t>
+  </si>
+  <si>
+    <t>MWF04-13H1-27KH-WH-WH-TRM</t>
+  </si>
+  <si>
+    <t>MICRO WALL WASH FLANGE 4 CELL 13W 2700KH WHITE-WHITE-TRIM</t>
+  </si>
+  <si>
+    <t>RMA16024</t>
+  </si>
+  <si>
+    <t>RMA16023</t>
+  </si>
+  <si>
+    <t>USAI-2DLA1-WD1-RESWH-00</t>
+  </si>
+  <si>
+    <t>PINHOLE RD ADJ  BLACK BFFL 16W 3022KH 25° S WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA16022</t>
+  </si>
+  <si>
+    <t>RMA16021</t>
+  </si>
+  <si>
+    <t>RMA16020</t>
+  </si>
+  <si>
+    <t>RMA16019</t>
+  </si>
+  <si>
+    <t>B4RAF-16C3-30KH-T25-FTA-UNV-D6E-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 RD ADJ TRMD 16W CLASSIC 30K 90CRI 25° BEAM FTA HSG 120-277V ELDO 1% LIN DM</t>
+  </si>
+  <si>
+    <t>RMA16018</t>
+  </si>
+  <si>
+    <t>RMA16016</t>
+  </si>
+  <si>
+    <t>RMA16015</t>
+  </si>
+  <si>
+    <t>RMA16014</t>
+  </si>
+  <si>
+    <t>SP-030-50</t>
+  </si>
+  <si>
+    <t>BEVELED 2.0/2.1 RND 50DEG DL OPTIC REPLACEMENT KIT</t>
+  </si>
+  <si>
+    <t>RMA16013</t>
+  </si>
+  <si>
+    <t>RMA16012</t>
+  </si>
+  <si>
+    <t>RMA16011</t>
+  </si>
+  <si>
+    <t>SP-241-0700-19</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT-BEVELED BLOCK 16W 700mA 120V-DIML19</t>
+  </si>
+  <si>
+    <t>RMA16010</t>
+  </si>
+  <si>
+    <t>RMA16009</t>
+  </si>
+  <si>
+    <t>SP-257-0350-2</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT-MINI BASIC-15W 350mA DIML2 HT</t>
+  </si>
+  <si>
+    <t>RMA16008</t>
+  </si>
+  <si>
+    <t>RMA16007</t>
+  </si>
+  <si>
+    <t>RMA16006</t>
+  </si>
+  <si>
+    <t>RMA16005</t>
+  </si>
+  <si>
+    <t>RMA16004</t>
+  </si>
+  <si>
+    <t>LEM-232-00-6022KS</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT 6" BEVELED CSD CRI 6022KS</t>
+  </si>
+  <si>
+    <t>RMA16002</t>
+  </si>
+  <si>
+    <t>RMA16001</t>
+  </si>
+  <si>
+    <t>RMA16000</t>
+  </si>
+  <si>
+    <t>RMA15999</t>
+  </si>
+  <si>
+    <t>SP-143-1000-19</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT-BEVELED 2.1 RT 24W-1000ma-120V-DIML19-HT</t>
+  </si>
+  <si>
+    <t>RMA15998</t>
+  </si>
+  <si>
+    <t>RMA15997</t>
+  </si>
+  <si>
+    <t>RMA15996</t>
+  </si>
+  <si>
+    <t>SP-175-0700-1M</t>
+  </si>
+  <si>
+    <t>DRIVER ASM BEVELED WRGB- 32W 350/350/350/700mA 120V-277V NC/IC/CP 8 BIT MANUAL ADDRESSING DMX DIM-EL</t>
+  </si>
+  <si>
+    <t>SP-192-RJ</t>
+  </si>
+  <si>
+    <t>INTERFACE- DMX SIGNAL WRGB- RJ45</t>
+  </si>
+  <si>
+    <t>RMA15995</t>
+  </si>
+  <si>
+    <t>RMA15994</t>
+  </si>
+  <si>
+    <t>USAI-3DL-SPACK-S-FT-00</t>
+  </si>
+  <si>
+    <t>RECESS 3 SQUARE FT SPACKLE FRAME KIT</t>
+  </si>
+  <si>
+    <t>RMA15993</t>
+  </si>
+  <si>
+    <t>RMA15992</t>
+  </si>
+  <si>
+    <t>USAI-3DLD1-SPSWH-00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAVANT/USAI RECESS 3 DL SQR TRML SOLITE LENS WHITE TRM_x000D_
+</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>RMA15990</t>
+  </si>
+  <si>
+    <t>USAI-3DLD1-SMSBZ-00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAVANT/USAI RECESS 3 DNL SQR MILL SOLITE LENS STATUARY BRONZE TRM 00
+</t>
   </si>
 </sst>
 </file>
@@ -7183,10 +7761,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1362"/>
+  <dimension ref="A1:F1497"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1205" workbookViewId="0">
-      <selection activeCell="L1214" sqref="L1214"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1440" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1363" sqref="A1363:F1497"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34434,6 +35013,2706 @@
         <v>2041</v>
       </c>
     </row>
+    <row r="1363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1363" s="1" t="s">
+        <v>2264</v>
+      </c>
+      <c r="B1363" s="1" t="s">
+        <v>2265</v>
+      </c>
+      <c r="C1363" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1363" s="1" t="s">
+        <v>2266</v>
+      </c>
+      <c r="E1363" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1363" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1364" s="1" t="s">
+        <v>2268</v>
+      </c>
+      <c r="B1364" s="1" t="s">
+        <v>2269</v>
+      </c>
+      <c r="C1364" s="1">
+        <v>9</v>
+      </c>
+      <c r="D1364" s="1" t="s">
+        <v>2270</v>
+      </c>
+      <c r="E1364" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1364" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1365" s="1" t="s">
+        <v>2271</v>
+      </c>
+      <c r="B1365" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1365" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1365" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E1365" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1365" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1366" s="1" t="s">
+        <v>2271</v>
+      </c>
+      <c r="B1366" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C1366" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1366" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E1366" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1366" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1367" s="1" t="s">
+        <v>2272</v>
+      </c>
+      <c r="B1367" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="C1367" s="1">
+        <v>8</v>
+      </c>
+      <c r="D1367" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="E1367" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1367" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1368" s="1" t="s">
+        <v>2273</v>
+      </c>
+      <c r="B1368" s="1" t="s">
+        <v>2274</v>
+      </c>
+      <c r="C1368" s="1">
+        <v>19</v>
+      </c>
+      <c r="D1368" s="1" t="s">
+        <v>2275</v>
+      </c>
+      <c r="E1368" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1368" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1369" s="1" t="s">
+        <v>2276</v>
+      </c>
+      <c r="B1369" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="C1369" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1369" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="E1369" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1369" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1370" s="1" t="s">
+        <v>2277</v>
+      </c>
+      <c r="B1370" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="C1370" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1370" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="E1370" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1370" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1371" s="1" t="s">
+        <v>2278</v>
+      </c>
+      <c r="B1371" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="C1371" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1371" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="E1371" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1371" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1372" s="1" t="s">
+        <v>2278</v>
+      </c>
+      <c r="B1372" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1372" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1372" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1372" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1372" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1373" s="1" t="s">
+        <v>2279</v>
+      </c>
+      <c r="B1373" s="1" t="s">
+        <v>2280</v>
+      </c>
+      <c r="C1373" s="1">
+        <v>36</v>
+      </c>
+      <c r="D1373" s="1" t="s">
+        <v>2281</v>
+      </c>
+      <c r="E1373" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1373" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1374" s="1" t="s">
+        <v>2279</v>
+      </c>
+      <c r="B1374" s="1" t="s">
+        <v>2282</v>
+      </c>
+      <c r="C1374" s="1">
+        <v>36</v>
+      </c>
+      <c r="D1374" s="1" t="s">
+        <v>2283</v>
+      </c>
+      <c r="E1374" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1374" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1375" s="1" t="s">
+        <v>2284</v>
+      </c>
+      <c r="B1375" s="1" t="s">
+        <v>2138</v>
+      </c>
+      <c r="C1375" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1375" s="1" t="s">
+        <v>2139</v>
+      </c>
+      <c r="E1375" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1375" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1376" s="1" t="s">
+        <v>2284</v>
+      </c>
+      <c r="B1376" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="C1376" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1376" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="E1376" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1376" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1377" s="1" t="s">
+        <v>2285</v>
+      </c>
+      <c r="B1377" s="1" t="s">
+        <v>2286</v>
+      </c>
+      <c r="C1377" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1377" s="1" t="s">
+        <v>2287</v>
+      </c>
+      <c r="E1377" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1377" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1378" s="1" t="s">
+        <v>2288</v>
+      </c>
+      <c r="B1378" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1378" s="1">
+        <v>8</v>
+      </c>
+      <c r="D1378" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1378" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1378" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1379" s="1" t="s">
+        <v>2288</v>
+      </c>
+      <c r="B1379" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C1379" s="1">
+        <v>8</v>
+      </c>
+      <c r="D1379" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E1379" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1379" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1380" s="1" t="s">
+        <v>2289</v>
+      </c>
+      <c r="B1380" s="1" t="s">
+        <v>2290</v>
+      </c>
+      <c r="C1380" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1380" s="1" t="s">
+        <v>2291</v>
+      </c>
+      <c r="E1380" s="1" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1380" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1381" s="1" t="s">
+        <v>2292</v>
+      </c>
+      <c r="B1381" s="1" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C1381" s="1">
+        <v>10</v>
+      </c>
+      <c r="D1381" s="1" t="s">
+        <v>1713</v>
+      </c>
+      <c r="E1381" s="1" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1381" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1382" s="1" t="s">
+        <v>2293</v>
+      </c>
+      <c r="B1382" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1382" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1382" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1382" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1382" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1383" s="1" t="s">
+        <v>2294</v>
+      </c>
+      <c r="B1383" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1383" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1383" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1383" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1383" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1384" s="1" t="s">
+        <v>2295</v>
+      </c>
+      <c r="B1384" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C1384" s="1">
+        <v>5</v>
+      </c>
+      <c r="D1384" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E1384" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1384" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1385" s="1" t="s">
+        <v>2296</v>
+      </c>
+      <c r="B1385" s="1" t="s">
+        <v>2297</v>
+      </c>
+      <c r="C1385" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1385" s="1" t="s">
+        <v>2298</v>
+      </c>
+      <c r="E1385" s="1" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1385" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1386" s="1" t="s">
+        <v>2299</v>
+      </c>
+      <c r="B1386" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C1386" s="1">
+        <v>6</v>
+      </c>
+      <c r="D1386" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="E1386" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1386" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1387" s="1" t="s">
+        <v>2300</v>
+      </c>
+      <c r="B1387" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="C1387" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1387" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="E1387" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1387" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1388" s="1" t="s">
+        <v>2300</v>
+      </c>
+      <c r="B1388" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="C1388" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1388" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="E1388" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1388" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1389" s="1" t="s">
+        <v>2300</v>
+      </c>
+      <c r="B1389" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1389" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1389" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1389" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1389" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1390" s="1" t="s">
+        <v>2301</v>
+      </c>
+      <c r="B1390" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="C1390" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1390" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="E1390" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1390" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1391" s="1" t="s">
+        <v>2302</v>
+      </c>
+      <c r="B1391" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C1391" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1391" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="E1391" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1391" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1392" s="1" t="s">
+        <v>2303</v>
+      </c>
+      <c r="B1392" s="1" t="s">
+        <v>2304</v>
+      </c>
+      <c r="C1392" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1392" s="1" t="s">
+        <v>2305</v>
+      </c>
+      <c r="E1392" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1392" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1393" s="1" t="s">
+        <v>2306</v>
+      </c>
+      <c r="B1393" s="1" t="s">
+        <v>2307</v>
+      </c>
+      <c r="C1393" s="1">
+        <v>4</v>
+      </c>
+      <c r="D1393" s="1" t="s">
+        <v>2308</v>
+      </c>
+      <c r="E1393" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1393" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1394" s="1" t="s">
+        <v>2309</v>
+      </c>
+      <c r="B1394" s="1" t="s">
+        <v>2192</v>
+      </c>
+      <c r="C1394" s="1">
+        <v>9</v>
+      </c>
+      <c r="D1394" s="1" t="s">
+        <v>2193</v>
+      </c>
+      <c r="E1394" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1394" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1395" s="1" t="s">
+        <v>2309</v>
+      </c>
+      <c r="B1395" s="1" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C1395" s="1">
+        <v>9</v>
+      </c>
+      <c r="D1395" s="1" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E1395" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1395" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1396" s="1" t="s">
+        <v>2310</v>
+      </c>
+      <c r="B1396" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1396" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1396" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1396" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1396" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1397" s="1" t="s">
+        <v>2310</v>
+      </c>
+      <c r="B1397" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1397" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1397" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1397" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1397" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1398" s="1" t="s">
+        <v>2311</v>
+      </c>
+      <c r="B1398" s="1" t="s">
+        <v>2312</v>
+      </c>
+      <c r="C1398" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1398" s="1" t="s">
+        <v>2313</v>
+      </c>
+      <c r="E1398" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1398" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1399" s="1" t="s">
+        <v>2314</v>
+      </c>
+      <c r="B1399" s="1" t="s">
+        <v>2315</v>
+      </c>
+      <c r="C1399" s="1">
+        <v>4</v>
+      </c>
+      <c r="D1399" s="1" t="s">
+        <v>2316</v>
+      </c>
+      <c r="E1399" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1399" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1400" s="1" t="s">
+        <v>2317</v>
+      </c>
+      <c r="B1400" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="C1400" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1400" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="E1400" s="1" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1400" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1401" s="1" t="s">
+        <v>2318</v>
+      </c>
+      <c r="B1401" s="1" t="s">
+        <v>2319</v>
+      </c>
+      <c r="C1401" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1401" s="1" t="s">
+        <v>2320</v>
+      </c>
+      <c r="E1401" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1401" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1402" s="1" t="s">
+        <v>2321</v>
+      </c>
+      <c r="B1402" s="1" t="s">
+        <v>2322</v>
+      </c>
+      <c r="C1402" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1402" s="1" t="s">
+        <v>2323</v>
+      </c>
+      <c r="E1402" s="1" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1402" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1403" s="1" t="s">
+        <v>2321</v>
+      </c>
+      <c r="B1403" s="1" t="s">
+        <v>2324</v>
+      </c>
+      <c r="C1403" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1403" s="1" t="s">
+        <v>2325</v>
+      </c>
+      <c r="E1403" s="1" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1403" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1404" s="1" t="s">
+        <v>2326</v>
+      </c>
+      <c r="B1404" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1404" s="1">
+        <v>10</v>
+      </c>
+      <c r="D1404" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1404" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1404" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1405" s="1" t="s">
+        <v>2327</v>
+      </c>
+      <c r="B1405" s="1" t="s">
+        <v>2328</v>
+      </c>
+      <c r="C1405" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1405" s="1" t="s">
+        <v>2329</v>
+      </c>
+      <c r="E1405" s="1" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1405" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1406" s="1" t="s">
+        <v>2330</v>
+      </c>
+      <c r="B1406" s="1" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C1406" s="1">
+        <v>12</v>
+      </c>
+      <c r="D1406" s="1" t="s">
+        <v>1579</v>
+      </c>
+      <c r="E1406" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1406" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1407" s="1" t="s">
+        <v>2331</v>
+      </c>
+      <c r="B1407" s="1" t="s">
+        <v>2332</v>
+      </c>
+      <c r="C1407" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1407" s="1" t="s">
+        <v>2333</v>
+      </c>
+      <c r="E1407" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="F1407" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1408" s="1" t="s">
+        <v>2331</v>
+      </c>
+      <c r="B1408" s="1" t="s">
+        <v>2334</v>
+      </c>
+      <c r="C1408" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1408" s="1" t="s">
+        <v>2335</v>
+      </c>
+      <c r="E1408" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="F1408" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1409" s="1" t="s">
+        <v>2331</v>
+      </c>
+      <c r="B1409" s="1" t="s">
+        <v>2336</v>
+      </c>
+      <c r="C1409" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1409" s="1" t="s">
+        <v>2337</v>
+      </c>
+      <c r="E1409" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="F1409" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1410" s="1" t="s">
+        <v>2331</v>
+      </c>
+      <c r="B1410" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1410" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1410" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1410" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="F1410" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1411" s="1" t="s">
+        <v>2331</v>
+      </c>
+      <c r="B1411" s="1" t="s">
+        <v>2338</v>
+      </c>
+      <c r="C1411" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1411" s="1" t="s">
+        <v>2339</v>
+      </c>
+      <c r="E1411" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="F1411" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1412" s="1" t="s">
+        <v>2340</v>
+      </c>
+      <c r="B1412" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="C1412" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1412" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="E1412" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1412" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1413" s="1" t="s">
+        <v>2341</v>
+      </c>
+      <c r="B1413" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="C1413" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1413" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="E1413" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1413" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1414" s="1" t="s">
+        <v>2342</v>
+      </c>
+      <c r="B1414" s="1" t="s">
+        <v>2343</v>
+      </c>
+      <c r="C1414" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1414" s="1" t="s">
+        <v>2344</v>
+      </c>
+      <c r="E1414" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1414" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1415" s="1" t="s">
+        <v>2345</v>
+      </c>
+      <c r="B1415" s="1" t="s">
+        <v>2044</v>
+      </c>
+      <c r="C1415" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1415" s="1" t="s">
+        <v>2045</v>
+      </c>
+      <c r="E1415" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1415" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1416" s="1" t="s">
+        <v>2346</v>
+      </c>
+      <c r="B1416" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="C1416" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1416" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="E1416" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1416" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1417" s="1" t="s">
+        <v>2347</v>
+      </c>
+      <c r="B1417" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1417" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1417" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1417" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1417" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1418" s="1" t="s">
+        <v>2348</v>
+      </c>
+      <c r="B1418" s="1" t="s">
+        <v>2349</v>
+      </c>
+      <c r="C1418" s="1">
+        <v>17</v>
+      </c>
+      <c r="D1418" s="1" t="s">
+        <v>2350</v>
+      </c>
+      <c r="E1418" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1418" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1419" s="1" t="s">
+        <v>2351</v>
+      </c>
+      <c r="B1419" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="C1419" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1419" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="E1419" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1419" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1420" s="1" t="s">
+        <v>2351</v>
+      </c>
+      <c r="B1420" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C1420" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1420" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="E1420" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1420" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1421" s="1" t="s">
+        <v>2352</v>
+      </c>
+      <c r="B1421" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="C1421" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1421" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="E1421" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1421" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1422" s="1" t="s">
+        <v>2353</v>
+      </c>
+      <c r="B1422" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1422" s="1">
+        <v>10</v>
+      </c>
+      <c r="D1422" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E1422" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1422" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1423" s="1" t="s">
+        <v>2353</v>
+      </c>
+      <c r="B1423" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1423" s="1">
+        <v>10</v>
+      </c>
+      <c r="D1423" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E1423" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1423" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1424" s="1" t="s">
+        <v>2353</v>
+      </c>
+      <c r="B1424" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C1424" s="1">
+        <v>10</v>
+      </c>
+      <c r="D1424" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E1424" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1424" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1425" s="1" t="s">
+        <v>2354</v>
+      </c>
+      <c r="B1425" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C1425" s="1">
+        <v>5</v>
+      </c>
+      <c r="D1425" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E1425" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1425" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1426" s="1" t="s">
+        <v>2355</v>
+      </c>
+      <c r="B1426" s="1" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C1426" s="1">
+        <v>4</v>
+      </c>
+      <c r="D1426" s="1" t="s">
+        <v>1107</v>
+      </c>
+      <c r="E1426" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1426" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1427" s="1" t="s">
+        <v>2356</v>
+      </c>
+      <c r="B1427" s="1" t="s">
+        <v>2357</v>
+      </c>
+      <c r="C1427" s="1">
+        <v>5</v>
+      </c>
+      <c r="D1427" s="1" t="s">
+        <v>2358</v>
+      </c>
+      <c r="E1427" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="F1427" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1428" s="1" t="s">
+        <v>2359</v>
+      </c>
+      <c r="B1428" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1428" s="1">
+        <v>4</v>
+      </c>
+      <c r="D1428" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1428" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1428" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1429" s="1" t="s">
+        <v>2360</v>
+      </c>
+      <c r="B1429" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1429" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1429" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1429" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1429" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1430" s="1" t="s">
+        <v>2361</v>
+      </c>
+      <c r="B1430" s="1" t="s">
+        <v>1736</v>
+      </c>
+      <c r="C1430" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1430" s="1" t="s">
+        <v>1737</v>
+      </c>
+      <c r="E1430" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1430" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1431" s="1" t="s">
+        <v>2362</v>
+      </c>
+      <c r="B1431" s="1" t="s">
+        <v>2363</v>
+      </c>
+      <c r="C1431" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1431" s="1" t="s">
+        <v>2364</v>
+      </c>
+      <c r="E1431" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1431" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1432" s="1" t="s">
+        <v>2362</v>
+      </c>
+      <c r="B1432" s="1" t="s">
+        <v>2365</v>
+      </c>
+      <c r="C1432" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1432" s="1" t="s">
+        <v>2366</v>
+      </c>
+      <c r="E1432" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1432" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1433" s="1" t="s">
+        <v>2367</v>
+      </c>
+      <c r="B1433" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1433" s="1">
+        <v>8</v>
+      </c>
+      <c r="D1433" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1433" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1433" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1434" s="1" t="s">
+        <v>2367</v>
+      </c>
+      <c r="B1434" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C1434" s="1">
+        <v>8</v>
+      </c>
+      <c r="D1434" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="E1434" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1434" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1435" s="1" t="s">
+        <v>2367</v>
+      </c>
+      <c r="B1435" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1435" s="1">
+        <v>4</v>
+      </c>
+      <c r="D1435" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1435" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1435" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1436" s="1" t="s">
+        <v>2367</v>
+      </c>
+      <c r="B1436" s="1" t="s">
+        <v>2004</v>
+      </c>
+      <c r="C1436" s="1">
+        <v>4</v>
+      </c>
+      <c r="D1436" s="1" t="s">
+        <v>2005</v>
+      </c>
+      <c r="E1436" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1436" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1437" s="1" t="s">
+        <v>2368</v>
+      </c>
+      <c r="B1437" s="1" t="s">
+        <v>2240</v>
+      </c>
+      <c r="C1437" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1437" s="1" t="s">
+        <v>2241</v>
+      </c>
+      <c r="E1437" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1437" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1438" s="1" t="s">
+        <v>2368</v>
+      </c>
+      <c r="B1438" s="1" t="s">
+        <v>2242</v>
+      </c>
+      <c r="C1438" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1438" s="1" t="s">
+        <v>2243</v>
+      </c>
+      <c r="E1438" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1438" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1439" s="1" t="s">
+        <v>2369</v>
+      </c>
+      <c r="B1439" s="1" t="s">
+        <v>2370</v>
+      </c>
+      <c r="C1439" s="1">
+        <v>8</v>
+      </c>
+      <c r="D1439" s="1" t="s">
+        <v>2371</v>
+      </c>
+      <c r="E1439" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1439" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1440" s="1" t="s">
+        <v>2372</v>
+      </c>
+      <c r="B1440" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="C1440" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1440" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="E1440" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1440" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1441" s="1" t="s">
+        <v>2373</v>
+      </c>
+      <c r="B1441" s="1" t="s">
+        <v>2374</v>
+      </c>
+      <c r="C1441" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1441" s="1" t="s">
+        <v>2375</v>
+      </c>
+      <c r="E1441" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1441" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1442" s="1" t="s">
+        <v>2376</v>
+      </c>
+      <c r="B1442" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="C1442" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1442" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="E1442" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1442" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1443" s="1" t="s">
+        <v>2376</v>
+      </c>
+      <c r="B1443" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="C1443" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1443" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="E1443" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1443" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1444" s="1" t="s">
+        <v>2377</v>
+      </c>
+      <c r="B1444" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1444" s="1">
+        <v>65</v>
+      </c>
+      <c r="D1444" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1444" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1444" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1445" s="1" t="s">
+        <v>2378</v>
+      </c>
+      <c r="B1445" s="1" t="s">
+        <v>2379</v>
+      </c>
+      <c r="C1445" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1445" s="1" t="s">
+        <v>2380</v>
+      </c>
+      <c r="E1445" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1445" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1446" s="1" t="s">
+        <v>2381</v>
+      </c>
+      <c r="B1446" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1446" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1446" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1446" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1446" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1447" s="1" t="s">
+        <v>2382</v>
+      </c>
+      <c r="B1447" s="1" t="s">
+        <v>2383</v>
+      </c>
+      <c r="C1447" s="1">
+        <v>5</v>
+      </c>
+      <c r="D1447" s="1" t="s">
+        <v>2384</v>
+      </c>
+      <c r="E1447" s="1" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F1447" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1448" s="1" t="s">
+        <v>2382</v>
+      </c>
+      <c r="B1448" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1448" s="1">
+        <v>5</v>
+      </c>
+      <c r="D1448" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1448" s="1" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F1448" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1449" s="1" t="s">
+        <v>2385</v>
+      </c>
+      <c r="B1449" s="1" t="s">
+        <v>2386</v>
+      </c>
+      <c r="C1449" s="1">
+        <v>4</v>
+      </c>
+      <c r="D1449" s="1" t="s">
+        <v>2387</v>
+      </c>
+      <c r="E1449" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1449" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1450" s="1" t="s">
+        <v>2388</v>
+      </c>
+      <c r="B1450" s="1" t="s">
+        <v>2389</v>
+      </c>
+      <c r="C1450" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1450" s="1" t="s">
+        <v>2390</v>
+      </c>
+      <c r="E1450" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="F1450" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1451" s="1" t="s">
+        <v>2391</v>
+      </c>
+      <c r="B1451" s="1" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C1451" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1451" s="1" t="s">
+        <v>1936</v>
+      </c>
+      <c r="E1451" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1451" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1452" s="1" t="s">
+        <v>2392</v>
+      </c>
+      <c r="B1452" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C1452" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1452" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1452" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1452" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1453" s="1" t="s">
+        <v>2393</v>
+      </c>
+      <c r="B1453" s="1" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C1453" s="1">
+        <v>10</v>
+      </c>
+      <c r="D1453" s="1" t="s">
+        <v>1619</v>
+      </c>
+      <c r="E1453" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1453" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1454" s="1" t="s">
+        <v>2394</v>
+      </c>
+      <c r="B1454" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="C1454" s="1">
+        <v>4</v>
+      </c>
+      <c r="D1454" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="E1454" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1454" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1455" s="1" t="s">
+        <v>2395</v>
+      </c>
+      <c r="B1455" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1455" s="1">
+        <v>17</v>
+      </c>
+      <c r="D1455" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="E1455" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1455" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1456" s="1" t="s">
+        <v>2396</v>
+      </c>
+      <c r="B1456" s="1" t="s">
+        <v>2397</v>
+      </c>
+      <c r="C1456" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1456" s="1" t="s">
+        <v>2398</v>
+      </c>
+      <c r="E1456" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1456" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1457" s="1" t="s">
+        <v>2399</v>
+      </c>
+      <c r="B1457" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1457" s="1">
+        <v>30</v>
+      </c>
+      <c r="D1457" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1457" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1457" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1458" s="1" t="s">
+        <v>2400</v>
+      </c>
+      <c r="B1458" s="1" t="s">
+        <v>2401</v>
+      </c>
+      <c r="C1458" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1458" s="1" t="s">
+        <v>2402</v>
+      </c>
+      <c r="E1458" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1458" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1459" s="1" t="s">
+        <v>2403</v>
+      </c>
+      <c r="B1459" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1459" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1459" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1459" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1459" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1460" s="1" t="s">
+        <v>2404</v>
+      </c>
+      <c r="B1460" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1460" s="1">
+        <v>32</v>
+      </c>
+      <c r="D1460" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1460" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1460" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1461" s="1" t="s">
+        <v>2405</v>
+      </c>
+      <c r="B1461" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="C1461" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1461" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="E1461" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1461" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1462" s="1" t="s">
+        <v>2405</v>
+      </c>
+      <c r="B1462" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C1462" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1462" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="E1462" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1462" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1463" s="1" t="s">
+        <v>2406</v>
+      </c>
+      <c r="B1463" s="1" t="s">
+        <v>2407</v>
+      </c>
+      <c r="C1463" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1463" s="1" t="s">
+        <v>2408</v>
+      </c>
+      <c r="E1463" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="F1463" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1464" s="1" t="s">
+        <v>2409</v>
+      </c>
+      <c r="B1464" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1464" s="1">
+        <v>20</v>
+      </c>
+      <c r="D1464" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1464" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1464" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1465" s="1" t="s">
+        <v>2410</v>
+      </c>
+      <c r="B1465" s="1" t="s">
+        <v>1426</v>
+      </c>
+      <c r="C1465" s="1">
+        <v>5</v>
+      </c>
+      <c r="D1465" s="1" t="s">
+        <v>1427</v>
+      </c>
+      <c r="E1465" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1465" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1466" s="1" t="s">
+        <v>2410</v>
+      </c>
+      <c r="B1466" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1466" s="1">
+        <v>5</v>
+      </c>
+      <c r="D1466" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1466" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1466" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1467" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="B1467" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1467" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1467" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1467" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1467" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1468" s="1" t="s">
+        <v>2411</v>
+      </c>
+      <c r="B1468" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1468" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1468" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1468" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1468" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1469" s="1" t="s">
+        <v>2412</v>
+      </c>
+      <c r="B1469" s="1" t="s">
+        <v>2413</v>
+      </c>
+      <c r="C1469" s="1">
+        <v>20</v>
+      </c>
+      <c r="D1469" s="1" t="s">
+        <v>2414</v>
+      </c>
+      <c r="E1469" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1469" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1470" s="1" t="s">
+        <v>2415</v>
+      </c>
+      <c r="B1470" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="C1470" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1470" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="E1470" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1470" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1471" s="1" t="s">
+        <v>2416</v>
+      </c>
+      <c r="B1471" s="1" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C1471" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1471" s="1" t="s">
+        <v>1619</v>
+      </c>
+      <c r="E1471" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1471" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1472" s="1" t="s">
+        <v>2417</v>
+      </c>
+      <c r="B1472" s="1" t="s">
+        <v>2418</v>
+      </c>
+      <c r="C1472" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1472" s="1" t="s">
+        <v>2419</v>
+      </c>
+      <c r="E1472" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1472" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1473" s="1" t="s">
+        <v>2420</v>
+      </c>
+      <c r="B1473" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1473" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1473" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1473" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1473" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1474" s="1" t="s">
+        <v>2421</v>
+      </c>
+      <c r="B1474" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1474" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1474" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1474" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1474" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1475" s="1" t="s">
+        <v>2421</v>
+      </c>
+      <c r="B1475" s="1" t="s">
+        <v>2422</v>
+      </c>
+      <c r="C1475" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1475" s="1" t="s">
+        <v>2423</v>
+      </c>
+      <c r="E1475" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1475" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1476" s="1" t="s">
+        <v>2424</v>
+      </c>
+      <c r="B1476" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1476" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1476" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1476" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1476" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1477" s="1" t="s">
+        <v>2425</v>
+      </c>
+      <c r="B1477" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1477" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1477" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="E1477" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1477" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1478" s="1" t="s">
+        <v>2426</v>
+      </c>
+      <c r="B1478" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1478" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1478" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1478" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1478" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1479" s="1" t="s">
+        <v>2427</v>
+      </c>
+      <c r="B1479" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="C1479" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1479" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="E1479" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1479" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1480" s="1" t="s">
+        <v>2428</v>
+      </c>
+      <c r="B1480" s="1" t="s">
+        <v>2429</v>
+      </c>
+      <c r="C1480" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1480" s="1" t="s">
+        <v>2430</v>
+      </c>
+      <c r="E1480" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1480" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1481" s="1" t="s">
+        <v>2431</v>
+      </c>
+      <c r="B1481" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="C1481" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1481" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="E1481" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1481" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1482" s="1" t="s">
+        <v>2432</v>
+      </c>
+      <c r="B1482" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="C1482" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1482" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="E1482" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1482" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1483" s="1" t="s">
+        <v>2433</v>
+      </c>
+      <c r="B1483" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1483" s="1">
+        <v>10</v>
+      </c>
+      <c r="D1483" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1483" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1483" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1484" s="1" t="s">
+        <v>2434</v>
+      </c>
+      <c r="B1484" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1484" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1484" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1484" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1484" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1485" s="1" t="s">
+        <v>2434</v>
+      </c>
+      <c r="B1485" s="1" t="s">
+        <v>2435</v>
+      </c>
+      <c r="C1485" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1485" s="1" t="s">
+        <v>2436</v>
+      </c>
+      <c r="E1485" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1485" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1486" s="1" t="s">
+        <v>2437</v>
+      </c>
+      <c r="B1486" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="C1486" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1486" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="E1486" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1486" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1487" s="1" t="s">
+        <v>2438</v>
+      </c>
+      <c r="B1487" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1487" s="1">
+        <v>9</v>
+      </c>
+      <c r="D1487" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1487" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1487" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1488" s="1" t="s">
+        <v>2438</v>
+      </c>
+      <c r="B1488" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="C1488" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1488" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="E1488" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1488" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1489" s="1" t="s">
+        <v>2439</v>
+      </c>
+      <c r="B1489" s="1" t="s">
+        <v>2440</v>
+      </c>
+      <c r="C1489" s="1">
+        <v>4</v>
+      </c>
+      <c r="D1489" s="1" t="s">
+        <v>2441</v>
+      </c>
+      <c r="E1489" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1489" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1490" s="1" t="s">
+        <v>2439</v>
+      </c>
+      <c r="B1490" s="1" t="s">
+        <v>2442</v>
+      </c>
+      <c r="C1490" s="1">
+        <v>4</v>
+      </c>
+      <c r="D1490" s="1" t="s">
+        <v>2443</v>
+      </c>
+      <c r="E1490" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1490" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1491" s="1" t="s">
+        <v>2444</v>
+      </c>
+      <c r="B1491" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1491" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1491" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1491" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1491" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1492" s="1" t="s">
+        <v>2445</v>
+      </c>
+      <c r="B1492" s="1" t="s">
+        <v>2446</v>
+      </c>
+      <c r="C1492" s="1">
+        <v>6</v>
+      </c>
+      <c r="D1492" s="1" t="s">
+        <v>2447</v>
+      </c>
+      <c r="E1492" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1492" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1493" s="1" t="s">
+        <v>2448</v>
+      </c>
+      <c r="B1493" s="1" t="s">
+        <v>1669</v>
+      </c>
+      <c r="C1493" s="1">
+        <v>10</v>
+      </c>
+      <c r="D1493" s="1" t="s">
+        <v>1670</v>
+      </c>
+      <c r="E1493" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1493" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1494" s="1" t="s">
+        <v>2449</v>
+      </c>
+      <c r="B1494" s="1" t="s">
+        <v>2450</v>
+      </c>
+      <c r="C1494" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1494" s="1" t="s">
+        <v>2451</v>
+      </c>
+      <c r="E1494" s="1" t="s">
+        <v>2452</v>
+      </c>
+      <c r="F1494" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1495" s="1" t="s">
+        <v>2449</v>
+      </c>
+      <c r="B1495" s="1" t="s">
+        <v>2450</v>
+      </c>
+      <c r="C1495" s="1">
+        <v>6</v>
+      </c>
+      <c r="D1495" s="1" t="s">
+        <v>2451</v>
+      </c>
+      <c r="E1495" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1495" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1496" s="1" t="s">
+        <v>2453</v>
+      </c>
+      <c r="B1496" s="1" t="s">
+        <v>2454</v>
+      </c>
+      <c r="C1496" s="1">
+        <v>9</v>
+      </c>
+      <c r="D1496" s="1" t="s">
+        <v>2455</v>
+      </c>
+      <c r="E1496" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1496" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1497" s="1" t="s">
+        <v>2453</v>
+      </c>
+      <c r="B1497" s="1" t="s">
+        <v>2450</v>
+      </c>
+      <c r="C1497" s="1">
+        <v>70</v>
+      </c>
+      <c r="D1497" s="1" t="s">
+        <v>2451</v>
+      </c>
+      <c r="E1497" s="1" t="s">
+        <v>2452</v>
+      </c>
+      <c r="F1497" s="2" t="s">
+        <v>2267</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Updated the YTD sales orders
</commit_message>
<xml_diff>
--- a/Code/Failure_rate/2021/YTD/2021_YTD.xlsx
+++ b/Code/Failure_rate/2021/YTD/2021_YTD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\project_files\USAI\Code\Failure_rate\2021\YTD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC4F773-A0B5-4EA2-9200-0C69113CD0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F7785A-2B75-4C40-BDEF-91AC0F418FF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="20550" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="20550" windowHeight="11790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8300" uniqueCount="2664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9030" uniqueCount="2863">
   <si>
     <t>RMA_ID</t>
   </si>
@@ -8020,6 +8020,603 @@
   </si>
   <si>
     <t>RMA16100</t>
+  </si>
+  <si>
+    <t>RMA16326</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>RMA16325</t>
+  </si>
+  <si>
+    <t>CM 27</t>
+  </si>
+  <si>
+    <t>27 INCH  CHANNEL BARS/2 BEVELED MINI FT</t>
+  </si>
+  <si>
+    <t>RMA16324</t>
+  </si>
+  <si>
+    <t>B4RWL-D2-WH-TRM</t>
+  </si>
+  <si>
+    <t>BEVELED ROUND TRML WW 5555 LENS DIFFUSION WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA16323</t>
+  </si>
+  <si>
+    <t>SP-062-0500-3</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT BEVELED BASIC NCSM  HSG 20WATT 500mA 120V DIML3-LU</t>
+  </si>
+  <si>
+    <t>RMA16322</t>
+  </si>
+  <si>
+    <t>7862-28</t>
+  </si>
+  <si>
+    <t>SLIVER MR16- 5" DL-3/8"-METALIZED GREY</t>
+  </si>
+  <si>
+    <t>RMA16321</t>
+  </si>
+  <si>
+    <t>SP-140-1400-6A</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT - BEVELED 2.1 NC/IC/CP 33WATT 1400mA 120V-277V-DIML6A EL</t>
+  </si>
+  <si>
+    <t>RMA16319</t>
+  </si>
+  <si>
+    <t>RMA16318</t>
+  </si>
+  <si>
+    <t>RMA16317</t>
+  </si>
+  <si>
+    <t>RMA16316</t>
+  </si>
+  <si>
+    <t>RMA16315</t>
+  </si>
+  <si>
+    <t>RMA16314</t>
+  </si>
+  <si>
+    <t>SP-140-1000-4</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT - BEVELED 2.1 NC/IC/CP 24 WATT 1000mA 120V-277V DIML4 LU</t>
+  </si>
+  <si>
+    <t>RMA16313</t>
+  </si>
+  <si>
+    <t>RMA16312</t>
+  </si>
+  <si>
+    <t>RMA16311</t>
+  </si>
+  <si>
+    <t>RMA16310</t>
+  </si>
+  <si>
+    <t>SV-X115-NC-UNV-D6F</t>
+  </si>
+  <si>
+    <t>SLIVERLED SQ/RND TRIMMED 15W NEW CONSTRUCTION HSG 120-277V-DIML6F</t>
+  </si>
+  <si>
+    <t>RMA16309</t>
+  </si>
+  <si>
+    <t>RPB-01-20WG2-UNV-D4P</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER MINI/NANO-1 FIXTURE MAX-20W WG2 500mA 120-277V D4P</t>
+  </si>
+  <si>
+    <t>RMA16307</t>
+  </si>
+  <si>
+    <t>CMRW8-20X3-35KS-W2-D1-BL-PJ1-120V-D22</t>
+  </si>
+  <si>
+    <t>BEVELED MINI CYL RD WW 20W BLACK 8" 3500KS W2 D1 PJ1 120V DIML22</t>
+  </si>
+  <si>
+    <t>SK-070-22</t>
+  </si>
+  <si>
+    <t>SAMPLE DIMMER-DIML22</t>
+  </si>
+  <si>
+    <t>PXA-24-BL</t>
+  </si>
+  <si>
+    <t>PENDANT MOUNT P1-24" BLACK FIELD CUTTABLE STEM</t>
+  </si>
+  <si>
+    <t>RMA16306</t>
+  </si>
+  <si>
+    <t>B3SDL-15L2-30KH-30-EC-120V-D21-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI SQ DL TRML 15W BASIC 30K 90CRI 30° BEAM EC HSG 120V D21</t>
+  </si>
+  <si>
+    <t>SK-070-21</t>
+  </si>
+  <si>
+    <t>SAMPLE DIMMER-DIML21</t>
+  </si>
+  <si>
+    <t>RMA16305</t>
+  </si>
+  <si>
+    <t>RMA16304</t>
+  </si>
+  <si>
+    <t>USAI-2DL-LED-WD1XX-00</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT PINHOLE WGD HI CRI 3000-2200K</t>
+  </si>
+  <si>
+    <t>RMA16303</t>
+  </si>
+  <si>
+    <t>LEM-239-01-35KH</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT-BEVELED 2.2 ADJ 90+CRI 3500K-WIDE ARRAY</t>
+  </si>
+  <si>
+    <t>RMA16302</t>
+  </si>
+  <si>
+    <t>RMA16301</t>
+  </si>
+  <si>
+    <t>M1RDF-09X1M-30KS-35-M0-WH-WH-NC-TRM</t>
+  </si>
+  <si>
+    <t>LITTLEONES MICRO RD DL TRMD 9W 3000K 80 CRI 35° BEAM MICRO DIF LENS WHITE WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA16300</t>
+  </si>
+  <si>
+    <t>B4RWL-D2-BL-TRM</t>
+  </si>
+  <si>
+    <t>BEVELED ROUND TRML WW 50° LENS DIFFUSION BLACK TRIM</t>
+  </si>
+  <si>
+    <t>RMA16299</t>
+  </si>
+  <si>
+    <t>RMA16298</t>
+  </si>
+  <si>
+    <t>RMA16297</t>
+  </si>
+  <si>
+    <t>RMA16296</t>
+  </si>
+  <si>
+    <t>RMA16295</t>
+  </si>
+  <si>
+    <t>B3SAL-15WG2-3022KH-50-NCIC-UNV-D4P-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI SQ ADJ TRML 15W WARM GLOW 30-22K 90CRI 50° BEAM NCIC HSG 120-277V D4P LUTRON ECO 1%</t>
+  </si>
+  <si>
+    <t>RMA16294</t>
+  </si>
+  <si>
+    <t>RMA16293</t>
+  </si>
+  <si>
+    <t>RMA16292</t>
+  </si>
+  <si>
+    <t>E2-221A</t>
+  </si>
+  <si>
+    <t>ADELS 3/FEMALE PLUG WHITE AC 166-1 BU/3 WHITE</t>
+  </si>
+  <si>
+    <t>RMA16291</t>
+  </si>
+  <si>
+    <t>RMA16290</t>
+  </si>
+  <si>
+    <t>E2-752-AA</t>
+  </si>
+  <si>
+    <t>EM BATTERY PACK IOTA 7W 'A' CONFIGURATION</t>
+  </si>
+  <si>
+    <t>RMA16288</t>
+  </si>
+  <si>
+    <t>RMA16287</t>
+  </si>
+  <si>
+    <t>RMA16286</t>
+  </si>
+  <si>
+    <t>AL55N</t>
+  </si>
+  <si>
+    <t>SIZE N-ACCESSORY LENS MICRODIFFUSION 55 X 55° BEAM</t>
+  </si>
+  <si>
+    <t>RMA16285</t>
+  </si>
+  <si>
+    <t>RMA16284</t>
+  </si>
+  <si>
+    <t>RMA16283</t>
+  </si>
+  <si>
+    <t>RMA16282</t>
+  </si>
+  <si>
+    <t>RMA16281</t>
+  </si>
+  <si>
+    <t>B3SDF-15X3-30KH-65-FT-RM-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED MINI SQ DL TRMD 15W CLASSIC 30K 90CRI 65° BEAM FT HSG RM</t>
+  </si>
+  <si>
+    <t>RMA16280</t>
+  </si>
+  <si>
+    <t>RMA16279</t>
+  </si>
+  <si>
+    <t>RMA16277</t>
+  </si>
+  <si>
+    <t>RMA16276</t>
+  </si>
+  <si>
+    <t>Z1RWF-15X1M-30KH-W2-NC-RM-HSG</t>
+  </si>
+  <si>
+    <t>ZEPTO RD WW TRMD 15W CLASSIC 30K 90CRI NADIR OPTIC NC HSG REMOTE POWER SUPPLY</t>
+  </si>
+  <si>
+    <t>RMA16275</t>
+  </si>
+  <si>
+    <t>SP-322-0350-3</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT DRIVER-REPLACEMENT MINI X1/X3/WG2/CS1 NC1/NCIC/NCCP-0350mA 120V-277V DIML3-TR</t>
+  </si>
+  <si>
+    <t>RMA16274</t>
+  </si>
+  <si>
+    <t>RMA16273</t>
+  </si>
+  <si>
+    <t>RMA16272</t>
+  </si>
+  <si>
+    <t>RMA16271</t>
+  </si>
+  <si>
+    <t>RMA16270</t>
+  </si>
+  <si>
+    <t>LEM-239-00-40KS</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT-BEVELED 2.2 ADJ 80+CRI 4000K-WIDE ARRAY</t>
+  </si>
+  <si>
+    <t>RMA16269</t>
+  </si>
+  <si>
+    <t>RMA16268</t>
+  </si>
+  <si>
+    <t>SP-187-X-15-D4H</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT CONNECT NC HSG 15W 350mA DIML4H-LU</t>
+  </si>
+  <si>
+    <t>RMA16267</t>
+  </si>
+  <si>
+    <t>RMA16266</t>
+  </si>
+  <si>
+    <t>RMA16265</t>
+  </si>
+  <si>
+    <t>M1SDL-09X1M-30KH-50-M0-WH-NC-TRM</t>
+  </si>
+  <si>
+    <t>LITTLEONES MICRO SQ DL TRML 9W 3000K 90 CRI 50° BEAM MICRO DIF LENS WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA16264</t>
+  </si>
+  <si>
+    <t>RMA16263</t>
+  </si>
+  <si>
+    <t>RMA16262</t>
+  </si>
+  <si>
+    <t>SK-098-B3SDP-GW-M1-B3SDP-WL-M15</t>
+  </si>
+  <si>
+    <t>USAI ARMSTRONG SAMPLE KIT SQ TRML TILE GUN METAL/SQ TRML TILE WHITE LUME</t>
+  </si>
+  <si>
+    <t>RMA16261</t>
+  </si>
+  <si>
+    <t>RMA16260</t>
+  </si>
+  <si>
+    <t>B4SDF-16C3-30KS-90-FTCP-UNV-D6E-HSG</t>
+  </si>
+  <si>
+    <t>BEVELED 2.2 SQ DL TRMD 16W CLASSIC 30K 80CRI 90° BEAM FTCP HSG 120-277V ELDO 1% LIN DIM</t>
+  </si>
+  <si>
+    <t>RMA16259</t>
+  </si>
+  <si>
+    <t>RMA16258</t>
+  </si>
+  <si>
+    <t>RMA16257</t>
+  </si>
+  <si>
+    <t>RMA16255</t>
+  </si>
+  <si>
+    <t>E2-016</t>
+  </si>
+  <si>
+    <t>THERMAL PROTECTOR 277</t>
+  </si>
+  <si>
+    <t>RMA16254</t>
+  </si>
+  <si>
+    <t>RMA16253</t>
+  </si>
+  <si>
+    <t>RMA16252</t>
+  </si>
+  <si>
+    <t>RMA16251</t>
+  </si>
+  <si>
+    <t>SP-033-0500-4</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT NANO MTG-2 20W-500mA 120V-277V DIML4-LU</t>
+  </si>
+  <si>
+    <t>RMA16250</t>
+  </si>
+  <si>
+    <t>RMA16248</t>
+  </si>
+  <si>
+    <t>LEM-275-32-2722KS</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT-BEVELED 2.2 WG2 32W 80CRI 2700-2200K</t>
+  </si>
+  <si>
+    <t>RMA16247</t>
+  </si>
+  <si>
+    <t>LEM-274-00-30KH</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT SLIVERLED HI CRI 3000K</t>
+  </si>
+  <si>
+    <t>SP-234-0700-28</t>
+  </si>
+  <si>
+    <t>DRIVER PLATE SLIVERLED 700mA-D28 WGD</t>
+  </si>
+  <si>
+    <t>RMA16246</t>
+  </si>
+  <si>
+    <t>RMA16245</t>
+  </si>
+  <si>
+    <t>RMA16244</t>
+  </si>
+  <si>
+    <t>LEM-274-00-35KS</t>
+  </si>
+  <si>
+    <t>LIGHT ENGINE MODULE REPLACEMENT SLIVERLED STD CRI 3500K</t>
+  </si>
+  <si>
+    <t>RMA16243</t>
+  </si>
+  <si>
+    <t>RPB-01-20X3-UNV-D6E-EM7</t>
+  </si>
+  <si>
+    <t>REMOTE DRIVER MINI/NANO-1 FIXTURE MAX-20W X3 500mA 120-277V D6E-EM 7W</t>
+  </si>
+  <si>
+    <t>RMA16242</t>
+  </si>
+  <si>
+    <t>RMA16241</t>
+  </si>
+  <si>
+    <t>SP-155-0350-2</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT- MINI NC1 14W 350mA 120V-277V-DIML2</t>
+  </si>
+  <si>
+    <t>RMA16240</t>
+  </si>
+  <si>
+    <t>RMA16239</t>
+  </si>
+  <si>
+    <t>RMA16238</t>
+  </si>
+  <si>
+    <t>RMA16237</t>
+  </si>
+  <si>
+    <t>SP-338-01-SQ-F-L</t>
+  </si>
+  <si>
+    <t>3" MINI COMPLETE NC1/NCIC/NC CCP SQUARE FLANGED TO FLANGELESS</t>
+  </si>
+  <si>
+    <t>B3SDL-S-AC-TRM</t>
+  </si>
+  <si>
+    <t>BEVELED MINI SQ DL/ADJ TRML SOLITE LENS -ANOD CLEAR MATTE BEVEL</t>
+  </si>
+  <si>
+    <t>B4RAL-25-S-AC-TRM</t>
+  </si>
+  <si>
+    <t>BEVELED ROUND TRML 0-25° ADJ SOLITE LENS CLEAR MATTE ANOD TRIM</t>
+  </si>
+  <si>
+    <t>RMA16236</t>
+  </si>
+  <si>
+    <t>M1RDL-09X1M-30KH-50-M0-WH-NC-TRM</t>
+  </si>
+  <si>
+    <t>LITTLEONES MICRO RD DL TRML 9W 3000K 90 CRI 50° BEAM MICRO DIF LENS WHITE TRIM</t>
+  </si>
+  <si>
+    <t>RMA16235</t>
+  </si>
+  <si>
+    <t>RMA16233</t>
+  </si>
+  <si>
+    <t>RMA16232</t>
+  </si>
+  <si>
+    <t>RMA16231</t>
+  </si>
+  <si>
+    <t>RMA16230</t>
+  </si>
+  <si>
+    <t>RMA16229</t>
+  </si>
+  <si>
+    <t>RMA16228</t>
+  </si>
+  <si>
+    <t>B4SCL-S-WH-TRM</t>
+  </si>
+  <si>
+    <t>BEVELED SQUARE TRML COMFORT SOLITE LENS WHITE</t>
+  </si>
+  <si>
+    <t>RMA16227</t>
+  </si>
+  <si>
+    <t>RMA16226</t>
+  </si>
+  <si>
+    <t>SP-140-0900-2</t>
+  </si>
+  <si>
+    <t>RMA16225</t>
+  </si>
+  <si>
+    <t>RMA16224</t>
+  </si>
+  <si>
+    <t>RMA16223</t>
+  </si>
+  <si>
+    <t>RMA16222</t>
+  </si>
+  <si>
+    <t>SP-189-0350-6E</t>
+  </si>
+  <si>
+    <t>DRIVER REPLACEMENT SLIVERLED 350mA-DIML6E-EL</t>
+  </si>
+  <si>
+    <t>RMA16221</t>
+  </si>
+  <si>
+    <t>RMA16220</t>
+  </si>
+  <si>
+    <t>RMA16219</t>
+  </si>
+  <si>
+    <t>MDL08-27H1-40KH-50-SM-TRM</t>
+  </si>
+  <si>
+    <t>MICRO DOWNLIGHT TRIMLESS 8 CELL 27W 4000K 90 CRI 50° SILVER MATTE TRIM</t>
+  </si>
+  <si>
+    <t>RMA16218</t>
+  </si>
+  <si>
+    <t>RMA16217</t>
+  </si>
+  <si>
+    <t>RMA16216</t>
+  </si>
+  <si>
+    <t>RMA16215</t>
+  </si>
+  <si>
+    <t>RMA16214</t>
+  </si>
+  <si>
+    <t>CBRD10-33C3-35KH-25-SF-WH-AR3-UNV-D6E</t>
+  </si>
+  <si>
+    <t>2.2 CYLINDER RD DL 33W CW 3500KH 25° BEAM-SOLITE FROSTED-WHITE-AR MOUNT 96" 120-277V D6E</t>
+  </si>
+  <si>
+    <t>RMA16213</t>
   </si>
 </sst>
 </file>
@@ -8372,11 +8969,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1660"/>
+  <dimension ref="A1:F1806"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1299" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1497" sqref="E1497"/>
+      <pane ySplit="1" topLeftCell="A1667" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1661" sqref="A1661:F1806"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41584,6 +42181,2926 @@
         <v>2457</v>
       </c>
     </row>
+    <row r="1661" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1661" t="s">
+        <v>2664</v>
+      </c>
+      <c r="B1661" t="s">
+        <v>813</v>
+      </c>
+      <c r="C1661">
+        <v>1</v>
+      </c>
+      <c r="D1661" t="s">
+        <v>814</v>
+      </c>
+      <c r="E1661" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1661" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1662" t="s">
+        <v>2666</v>
+      </c>
+      <c r="B1662" t="s">
+        <v>2667</v>
+      </c>
+      <c r="C1662">
+        <v>24</v>
+      </c>
+      <c r="D1662" t="s">
+        <v>2668</v>
+      </c>
+      <c r="E1662" t="s">
+        <v>379</v>
+      </c>
+      <c r="F1662" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1663" t="s">
+        <v>2669</v>
+      </c>
+      <c r="B1663" t="s">
+        <v>2670</v>
+      </c>
+      <c r="C1663">
+        <v>2</v>
+      </c>
+      <c r="D1663" t="s">
+        <v>2671</v>
+      </c>
+      <c r="E1663" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1663" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1664" t="s">
+        <v>2672</v>
+      </c>
+      <c r="B1664" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C1664">
+        <v>2</v>
+      </c>
+      <c r="D1664" t="s">
+        <v>1518</v>
+      </c>
+      <c r="E1664" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1664" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1665" t="s">
+        <v>2672</v>
+      </c>
+      <c r="B1665" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1665">
+        <v>2</v>
+      </c>
+      <c r="D1665" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1665" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1665" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1666" t="s">
+        <v>2672</v>
+      </c>
+      <c r="B1666" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1666">
+        <v>1</v>
+      </c>
+      <c r="D1666" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1666" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1666" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1667" t="s">
+        <v>2672</v>
+      </c>
+      <c r="B1667" t="s">
+        <v>2673</v>
+      </c>
+      <c r="C1667">
+        <v>1</v>
+      </c>
+      <c r="D1667" t="s">
+        <v>2674</v>
+      </c>
+      <c r="E1667" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1667" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1668" t="s">
+        <v>2675</v>
+      </c>
+      <c r="B1668" t="s">
+        <v>2676</v>
+      </c>
+      <c r="C1668">
+        <v>1</v>
+      </c>
+      <c r="D1668" t="s">
+        <v>2677</v>
+      </c>
+      <c r="E1668" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1668" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1669" t="s">
+        <v>2678</v>
+      </c>
+      <c r="B1669" t="s">
+        <v>2679</v>
+      </c>
+      <c r="C1669">
+        <v>6</v>
+      </c>
+      <c r="D1669" t="s">
+        <v>2680</v>
+      </c>
+      <c r="E1669" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1669" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1670" t="s">
+        <v>2678</v>
+      </c>
+      <c r="B1670" t="s">
+        <v>836</v>
+      </c>
+      <c r="C1670">
+        <v>6</v>
+      </c>
+      <c r="D1670" t="s">
+        <v>837</v>
+      </c>
+      <c r="E1670" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1670" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1671" t="s">
+        <v>2681</v>
+      </c>
+      <c r="B1671" t="s">
+        <v>472</v>
+      </c>
+      <c r="C1671">
+        <v>1</v>
+      </c>
+      <c r="D1671" t="s">
+        <v>473</v>
+      </c>
+      <c r="E1671" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1671" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1672" t="s">
+        <v>2682</v>
+      </c>
+      <c r="B1672" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C1672">
+        <v>1</v>
+      </c>
+      <c r="D1672" t="s">
+        <v>1518</v>
+      </c>
+      <c r="E1672" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1672" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1673" t="s">
+        <v>2683</v>
+      </c>
+      <c r="B1673" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1673">
+        <v>1</v>
+      </c>
+      <c r="D1673" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1673" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1673" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1674" t="s">
+        <v>2684</v>
+      </c>
+      <c r="B1674" t="s">
+        <v>2440</v>
+      </c>
+      <c r="C1674">
+        <v>5</v>
+      </c>
+      <c r="D1674" t="s">
+        <v>2441</v>
+      </c>
+      <c r="E1674" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1674" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1675" t="s">
+        <v>2684</v>
+      </c>
+      <c r="B1675" t="s">
+        <v>2440</v>
+      </c>
+      <c r="C1675">
+        <v>15</v>
+      </c>
+      <c r="D1675" t="s">
+        <v>2441</v>
+      </c>
+      <c r="E1675" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1675" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1676" t="s">
+        <v>2685</v>
+      </c>
+      <c r="B1676" t="s">
+        <v>417</v>
+      </c>
+      <c r="C1676">
+        <v>1</v>
+      </c>
+      <c r="D1676" t="s">
+        <v>418</v>
+      </c>
+      <c r="E1676" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1676" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1677" t="s">
+        <v>2686</v>
+      </c>
+      <c r="B1677" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1677">
+        <v>1</v>
+      </c>
+      <c r="D1677" t="s">
+        <v>317</v>
+      </c>
+      <c r="E1677" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1677" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1678" t="s">
+        <v>2686</v>
+      </c>
+      <c r="B1678" t="s">
+        <v>2687</v>
+      </c>
+      <c r="C1678">
+        <v>1</v>
+      </c>
+      <c r="D1678" t="s">
+        <v>2688</v>
+      </c>
+      <c r="E1678" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1678" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1679" t="s">
+        <v>2689</v>
+      </c>
+      <c r="B1679" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1679">
+        <v>2</v>
+      </c>
+      <c r="D1679" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1679" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1679" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1680" t="s">
+        <v>2689</v>
+      </c>
+      <c r="B1680" t="s">
+        <v>2639</v>
+      </c>
+      <c r="C1680">
+        <v>2</v>
+      </c>
+      <c r="D1680" t="s">
+        <v>2640</v>
+      </c>
+      <c r="E1680" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1680" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1681" t="s">
+        <v>2690</v>
+      </c>
+      <c r="B1681" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1681">
+        <v>1</v>
+      </c>
+      <c r="D1681" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1681" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1681" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1682" t="s">
+        <v>2691</v>
+      </c>
+      <c r="B1682" t="s">
+        <v>492</v>
+      </c>
+      <c r="C1682">
+        <v>1</v>
+      </c>
+      <c r="D1682" t="s">
+        <v>493</v>
+      </c>
+      <c r="E1682" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1682" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1683" t="s">
+        <v>2692</v>
+      </c>
+      <c r="B1683" t="s">
+        <v>2693</v>
+      </c>
+      <c r="C1683">
+        <v>78</v>
+      </c>
+      <c r="D1683" t="s">
+        <v>2694</v>
+      </c>
+      <c r="E1683" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1683" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1684" t="s">
+        <v>2695</v>
+      </c>
+      <c r="B1684" t="s">
+        <v>2696</v>
+      </c>
+      <c r="C1684">
+        <v>1</v>
+      </c>
+      <c r="D1684" t="s">
+        <v>2697</v>
+      </c>
+      <c r="E1684" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1684" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1685" t="s">
+        <v>2698</v>
+      </c>
+      <c r="B1685" t="s">
+        <v>2699</v>
+      </c>
+      <c r="C1685">
+        <v>2</v>
+      </c>
+      <c r="D1685" t="s">
+        <v>2700</v>
+      </c>
+      <c r="E1685" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1685" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1686" t="s">
+        <v>2698</v>
+      </c>
+      <c r="B1686" t="s">
+        <v>2701</v>
+      </c>
+      <c r="C1686">
+        <v>2</v>
+      </c>
+      <c r="D1686" t="s">
+        <v>2702</v>
+      </c>
+      <c r="E1686" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1686" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1687" t="s">
+        <v>2698</v>
+      </c>
+      <c r="B1687" t="s">
+        <v>2703</v>
+      </c>
+      <c r="C1687">
+        <v>2</v>
+      </c>
+      <c r="D1687" t="s">
+        <v>2704</v>
+      </c>
+      <c r="E1687" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1687" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1688" t="s">
+        <v>2705</v>
+      </c>
+      <c r="B1688" t="s">
+        <v>2706</v>
+      </c>
+      <c r="C1688">
+        <v>1</v>
+      </c>
+      <c r="D1688" t="s">
+        <v>2707</v>
+      </c>
+      <c r="E1688" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1688" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1689" t="s">
+        <v>2705</v>
+      </c>
+      <c r="B1689" t="s">
+        <v>2708</v>
+      </c>
+      <c r="C1689">
+        <v>1</v>
+      </c>
+      <c r="D1689" t="s">
+        <v>2709</v>
+      </c>
+      <c r="E1689" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1689" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1690" t="s">
+        <v>2710</v>
+      </c>
+      <c r="B1690" t="s">
+        <v>2628</v>
+      </c>
+      <c r="C1690">
+        <v>2</v>
+      </c>
+      <c r="D1690" t="s">
+        <v>2629</v>
+      </c>
+      <c r="E1690" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1690" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1691" t="s">
+        <v>2711</v>
+      </c>
+      <c r="B1691" t="s">
+        <v>2712</v>
+      </c>
+      <c r="C1691">
+        <v>2</v>
+      </c>
+      <c r="D1691" t="s">
+        <v>2713</v>
+      </c>
+      <c r="E1691" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1691" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1692" t="s">
+        <v>2714</v>
+      </c>
+      <c r="B1692" t="s">
+        <v>2715</v>
+      </c>
+      <c r="C1692">
+        <v>1</v>
+      </c>
+      <c r="D1692" t="s">
+        <v>2716</v>
+      </c>
+      <c r="E1692" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1692" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1693" t="s">
+        <v>2714</v>
+      </c>
+      <c r="B1693" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C1693">
+        <v>1</v>
+      </c>
+      <c r="D1693" t="s">
+        <v>1518</v>
+      </c>
+      <c r="E1693" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1693" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1694" t="s">
+        <v>2717</v>
+      </c>
+      <c r="B1694" t="s">
+        <v>600</v>
+      </c>
+      <c r="C1694">
+        <v>1</v>
+      </c>
+      <c r="D1694" t="s">
+        <v>601</v>
+      </c>
+      <c r="E1694" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1694" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1695" t="s">
+        <v>2718</v>
+      </c>
+      <c r="B1695" t="s">
+        <v>2719</v>
+      </c>
+      <c r="C1695">
+        <v>2</v>
+      </c>
+      <c r="D1695" t="s">
+        <v>2720</v>
+      </c>
+      <c r="E1695" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1695" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1696" t="s">
+        <v>2721</v>
+      </c>
+      <c r="B1696" t="s">
+        <v>2722</v>
+      </c>
+      <c r="C1696">
+        <v>3</v>
+      </c>
+      <c r="D1696" t="s">
+        <v>2723</v>
+      </c>
+      <c r="E1696" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1696" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1697" t="s">
+        <v>2724</v>
+      </c>
+      <c r="B1697" t="s">
+        <v>816</v>
+      </c>
+      <c r="C1697">
+        <v>7</v>
+      </c>
+      <c r="D1697" t="s">
+        <v>817</v>
+      </c>
+      <c r="E1697" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1697" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1698" t="s">
+        <v>2725</v>
+      </c>
+      <c r="B1698" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C1698">
+        <v>2</v>
+      </c>
+      <c r="D1698" t="s">
+        <v>1840</v>
+      </c>
+      <c r="E1698" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1698" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1699" t="s">
+        <v>2726</v>
+      </c>
+      <c r="B1699" t="s">
+        <v>343</v>
+      </c>
+      <c r="C1699">
+        <v>7</v>
+      </c>
+      <c r="D1699" t="s">
+        <v>344</v>
+      </c>
+      <c r="E1699" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1699" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1700" t="s">
+        <v>2726</v>
+      </c>
+      <c r="B1700" t="s">
+        <v>774</v>
+      </c>
+      <c r="C1700">
+        <v>7</v>
+      </c>
+      <c r="D1700" t="s">
+        <v>775</v>
+      </c>
+      <c r="E1700" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1700" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1701" t="s">
+        <v>2727</v>
+      </c>
+      <c r="B1701" t="s">
+        <v>2222</v>
+      </c>
+      <c r="C1701">
+        <v>1</v>
+      </c>
+      <c r="D1701" t="s">
+        <v>2223</v>
+      </c>
+      <c r="E1701" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1701" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1702" t="s">
+        <v>2728</v>
+      </c>
+      <c r="B1702" t="s">
+        <v>2729</v>
+      </c>
+      <c r="C1702">
+        <v>1</v>
+      </c>
+      <c r="D1702" t="s">
+        <v>2730</v>
+      </c>
+      <c r="E1702" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1702" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1703" t="s">
+        <v>2731</v>
+      </c>
+      <c r="B1703" t="s">
+        <v>2631</v>
+      </c>
+      <c r="C1703">
+        <v>95</v>
+      </c>
+      <c r="D1703" t="s">
+        <v>2632</v>
+      </c>
+      <c r="E1703" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1703" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1704" t="s">
+        <v>2732</v>
+      </c>
+      <c r="B1704" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C1704">
+        <v>19</v>
+      </c>
+      <c r="D1704" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E1704" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1704" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1705" t="s">
+        <v>2733</v>
+      </c>
+      <c r="B1705" t="s">
+        <v>861</v>
+      </c>
+      <c r="C1705">
+        <v>1</v>
+      </c>
+      <c r="D1705" t="s">
+        <v>862</v>
+      </c>
+      <c r="E1705" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1705" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1706" t="s">
+        <v>2733</v>
+      </c>
+      <c r="B1706" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C1706">
+        <v>3</v>
+      </c>
+      <c r="D1706" t="s">
+        <v>1716</v>
+      </c>
+      <c r="E1706" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1706" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1707" t="s">
+        <v>2733</v>
+      </c>
+      <c r="B1707" t="s">
+        <v>2734</v>
+      </c>
+      <c r="C1707">
+        <v>4</v>
+      </c>
+      <c r="D1707" t="s">
+        <v>2735</v>
+      </c>
+      <c r="E1707" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1707" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1708" t="s">
+        <v>2736</v>
+      </c>
+      <c r="B1708" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C1708">
+        <v>1</v>
+      </c>
+      <c r="D1708" t="s">
+        <v>1728</v>
+      </c>
+      <c r="E1708" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1708" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1709" t="s">
+        <v>2737</v>
+      </c>
+      <c r="B1709" t="s">
+        <v>2738</v>
+      </c>
+      <c r="C1709">
+        <v>2</v>
+      </c>
+      <c r="D1709" t="s">
+        <v>2739</v>
+      </c>
+      <c r="E1709" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1709" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1710" t="s">
+        <v>2740</v>
+      </c>
+      <c r="B1710" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1710">
+        <v>6</v>
+      </c>
+      <c r="D1710" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1710" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1710" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1711" t="s">
+        <v>2741</v>
+      </c>
+      <c r="B1711" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1711">
+        <v>1</v>
+      </c>
+      <c r="D1711" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1711" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1711" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1712" t="s">
+        <v>2742</v>
+      </c>
+      <c r="B1712" t="s">
+        <v>2743</v>
+      </c>
+      <c r="C1712">
+        <v>23</v>
+      </c>
+      <c r="D1712" t="s">
+        <v>2744</v>
+      </c>
+      <c r="E1712" t="s">
+        <v>687</v>
+      </c>
+      <c r="F1712" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1713" t="s">
+        <v>2745</v>
+      </c>
+      <c r="B1713" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1713">
+        <v>3</v>
+      </c>
+      <c r="D1713" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1713" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1713" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1714" t="s">
+        <v>2745</v>
+      </c>
+      <c r="B1714" t="s">
+        <v>906</v>
+      </c>
+      <c r="C1714">
+        <v>1</v>
+      </c>
+      <c r="D1714" t="s">
+        <v>907</v>
+      </c>
+      <c r="E1714" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1714" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1715" t="s">
+        <v>2746</v>
+      </c>
+      <c r="B1715" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1715">
+        <v>1</v>
+      </c>
+      <c r="D1715" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1715" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1715" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1716" t="s">
+        <v>2747</v>
+      </c>
+      <c r="B1716" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1716">
+        <v>1</v>
+      </c>
+      <c r="D1716" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1716" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1716" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1717" t="s">
+        <v>2748</v>
+      </c>
+      <c r="B1717" t="s">
+        <v>943</v>
+      </c>
+      <c r="C1717">
+        <v>18</v>
+      </c>
+      <c r="D1717" t="s">
+        <v>944</v>
+      </c>
+      <c r="E1717" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1717" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1718" t="s">
+        <v>2749</v>
+      </c>
+      <c r="B1718" t="s">
+        <v>2750</v>
+      </c>
+      <c r="C1718">
+        <v>11</v>
+      </c>
+      <c r="D1718" t="s">
+        <v>2751</v>
+      </c>
+      <c r="E1718" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1718" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1719" t="s">
+        <v>2749</v>
+      </c>
+      <c r="B1719" t="s">
+        <v>2750</v>
+      </c>
+      <c r="C1719">
+        <v>30</v>
+      </c>
+      <c r="D1719" t="s">
+        <v>2751</v>
+      </c>
+      <c r="E1719" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1719" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1720" t="s">
+        <v>2752</v>
+      </c>
+      <c r="B1720" t="s">
+        <v>623</v>
+      </c>
+      <c r="C1720">
+        <v>1</v>
+      </c>
+      <c r="D1720" t="s">
+        <v>624</v>
+      </c>
+      <c r="E1720" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1720" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1721" t="s">
+        <v>2753</v>
+      </c>
+      <c r="B1721" t="s">
+        <v>816</v>
+      </c>
+      <c r="C1721">
+        <v>3</v>
+      </c>
+      <c r="D1721" t="s">
+        <v>817</v>
+      </c>
+      <c r="E1721" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1721" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1722" t="s">
+        <v>2753</v>
+      </c>
+      <c r="B1722" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1722">
+        <v>14</v>
+      </c>
+      <c r="D1722" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1722" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1722" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1723" t="s">
+        <v>2754</v>
+      </c>
+      <c r="B1723" t="s">
+        <v>458</v>
+      </c>
+      <c r="C1723">
+        <v>1</v>
+      </c>
+      <c r="D1723" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1723" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1723" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1724" t="s">
+        <v>2755</v>
+      </c>
+      <c r="B1724" t="s">
+        <v>2756</v>
+      </c>
+      <c r="C1724">
+        <v>1</v>
+      </c>
+      <c r="D1724" t="s">
+        <v>2757</v>
+      </c>
+      <c r="E1724" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1724" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1725" t="s">
+        <v>2758</v>
+      </c>
+      <c r="B1725" t="s">
+        <v>2759</v>
+      </c>
+      <c r="C1725">
+        <v>1</v>
+      </c>
+      <c r="D1725" t="s">
+        <v>2760</v>
+      </c>
+      <c r="E1725" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1725" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1726" t="s">
+        <v>2761</v>
+      </c>
+      <c r="B1726" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C1726">
+        <v>10</v>
+      </c>
+      <c r="D1726" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1726" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1726" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1727" t="s">
+        <v>2762</v>
+      </c>
+      <c r="B1727" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1727">
+        <v>4</v>
+      </c>
+      <c r="D1727" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1727" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1727" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1728" t="s">
+        <v>2763</v>
+      </c>
+      <c r="B1728" t="s">
+        <v>476</v>
+      </c>
+      <c r="C1728">
+        <v>1</v>
+      </c>
+      <c r="D1728" t="s">
+        <v>477</v>
+      </c>
+      <c r="E1728" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1728" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1729" t="s">
+        <v>2764</v>
+      </c>
+      <c r="B1729" t="s">
+        <v>1618</v>
+      </c>
+      <c r="C1729">
+        <v>1</v>
+      </c>
+      <c r="D1729" t="s">
+        <v>1619</v>
+      </c>
+      <c r="E1729" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1729" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1730" t="s">
+        <v>2764</v>
+      </c>
+      <c r="B1730" t="s">
+        <v>1485</v>
+      </c>
+      <c r="C1730">
+        <v>2</v>
+      </c>
+      <c r="D1730" t="s">
+        <v>1486</v>
+      </c>
+      <c r="E1730" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1730" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1731" t="s">
+        <v>2765</v>
+      </c>
+      <c r="B1731" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C1731">
+        <v>1</v>
+      </c>
+      <c r="D1731" t="s">
+        <v>1518</v>
+      </c>
+      <c r="E1731" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1731" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1732" t="s">
+        <v>2765</v>
+      </c>
+      <c r="B1732" t="s">
+        <v>2766</v>
+      </c>
+      <c r="C1732">
+        <v>1</v>
+      </c>
+      <c r="D1732" t="s">
+        <v>2767</v>
+      </c>
+      <c r="E1732" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1732" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1733" t="s">
+        <v>2768</v>
+      </c>
+      <c r="B1733" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1733">
+        <v>8</v>
+      </c>
+      <c r="D1733" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1733" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1733" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1734" t="s">
+        <v>2769</v>
+      </c>
+      <c r="B1734" t="s">
+        <v>2770</v>
+      </c>
+      <c r="C1734">
+        <v>2</v>
+      </c>
+      <c r="D1734" t="s">
+        <v>2771</v>
+      </c>
+      <c r="E1734" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1734" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1735" t="s">
+        <v>2772</v>
+      </c>
+      <c r="B1735" t="s">
+        <v>445</v>
+      </c>
+      <c r="C1735">
+        <v>4</v>
+      </c>
+      <c r="D1735" t="s">
+        <v>446</v>
+      </c>
+      <c r="E1735" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1735" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1736" t="s">
+        <v>2773</v>
+      </c>
+      <c r="B1736" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1736">
+        <v>20</v>
+      </c>
+      <c r="D1736" t="s">
+        <v>293</v>
+      </c>
+      <c r="E1736" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1736" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1737" t="s">
+        <v>2774</v>
+      </c>
+      <c r="B1737" t="s">
+        <v>2775</v>
+      </c>
+      <c r="C1737">
+        <v>12</v>
+      </c>
+      <c r="D1737" t="s">
+        <v>2776</v>
+      </c>
+      <c r="E1737" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1737" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1738" t="s">
+        <v>2777</v>
+      </c>
+      <c r="B1738" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1738">
+        <v>5</v>
+      </c>
+      <c r="D1738" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1738" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1738" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1739" t="s">
+        <v>2778</v>
+      </c>
+      <c r="B1739" t="s">
+        <v>760</v>
+      </c>
+      <c r="C1739">
+        <v>3</v>
+      </c>
+      <c r="D1739" t="s">
+        <v>761</v>
+      </c>
+      <c r="E1739" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1739" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1740" t="s">
+        <v>2779</v>
+      </c>
+      <c r="B1740" t="s">
+        <v>2780</v>
+      </c>
+      <c r="C1740">
+        <v>1</v>
+      </c>
+      <c r="D1740" t="s">
+        <v>2781</v>
+      </c>
+      <c r="E1740" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1740" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1741" t="s">
+        <v>2782</v>
+      </c>
+      <c r="B1741" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1741">
+        <v>10</v>
+      </c>
+      <c r="D1741" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1741" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1741" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1742" t="s">
+        <v>2782</v>
+      </c>
+      <c r="B1742" t="s">
+        <v>836</v>
+      </c>
+      <c r="C1742">
+        <v>5</v>
+      </c>
+      <c r="D1742" t="s">
+        <v>837</v>
+      </c>
+      <c r="E1742" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1742" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1743" t="s">
+        <v>2783</v>
+      </c>
+      <c r="B1743" t="s">
+        <v>2784</v>
+      </c>
+      <c r="C1743">
+        <v>2</v>
+      </c>
+      <c r="D1743" t="s">
+        <v>2785</v>
+      </c>
+      <c r="E1743" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1743" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1744" t="s">
+        <v>2786</v>
+      </c>
+      <c r="B1744" t="s">
+        <v>2297</v>
+      </c>
+      <c r="C1744">
+        <v>1</v>
+      </c>
+      <c r="D1744" t="s">
+        <v>2298</v>
+      </c>
+      <c r="E1744" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1744" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1745" t="s">
+        <v>2787</v>
+      </c>
+      <c r="B1745" t="s">
+        <v>2104</v>
+      </c>
+      <c r="C1745">
+        <v>12</v>
+      </c>
+      <c r="D1745" t="s">
+        <v>2105</v>
+      </c>
+      <c r="E1745" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1745" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1746" t="s">
+        <v>2788</v>
+      </c>
+      <c r="B1746" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C1746">
+        <v>1</v>
+      </c>
+      <c r="D1746" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E1746" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1746" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1747" t="s">
+        <v>2788</v>
+      </c>
+      <c r="B1747" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C1747">
+        <v>1</v>
+      </c>
+      <c r="D1747" t="s">
+        <v>1184</v>
+      </c>
+      <c r="E1747" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1747" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1748" t="s">
+        <v>2789</v>
+      </c>
+      <c r="B1748" t="s">
+        <v>2790</v>
+      </c>
+      <c r="C1748">
+        <v>6</v>
+      </c>
+      <c r="D1748" t="s">
+        <v>2791</v>
+      </c>
+      <c r="E1748" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1748" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1749" t="s">
+        <v>2792</v>
+      </c>
+      <c r="B1749" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1749">
+        <v>2</v>
+      </c>
+      <c r="D1749" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1749" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1749" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1750" t="s">
+        <v>2793</v>
+      </c>
+      <c r="B1750" t="s">
+        <v>458</v>
+      </c>
+      <c r="C1750">
+        <v>11</v>
+      </c>
+      <c r="D1750" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1750" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1750" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1751" t="s">
+        <v>2793</v>
+      </c>
+      <c r="B1751" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1751">
+        <v>11</v>
+      </c>
+      <c r="D1751" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1751" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1751" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1752" t="s">
+        <v>2794</v>
+      </c>
+      <c r="B1752" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1752">
+        <v>2</v>
+      </c>
+      <c r="D1752" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1752" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1752" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1753" t="s">
+        <v>2795</v>
+      </c>
+      <c r="B1753" t="s">
+        <v>2796</v>
+      </c>
+      <c r="C1753">
+        <v>2</v>
+      </c>
+      <c r="D1753" t="s">
+        <v>2797</v>
+      </c>
+      <c r="E1753" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1753" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1754" t="s">
+        <v>2795</v>
+      </c>
+      <c r="B1754" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1754">
+        <v>4</v>
+      </c>
+      <c r="D1754" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1754" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1754" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1755" t="s">
+        <v>2798</v>
+      </c>
+      <c r="B1755" t="s">
+        <v>626</v>
+      </c>
+      <c r="C1755">
+        <v>6</v>
+      </c>
+      <c r="D1755" t="s">
+        <v>627</v>
+      </c>
+      <c r="E1755" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F1755" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1756" t="s">
+        <v>2798</v>
+      </c>
+      <c r="B1756" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1756">
+        <v>3</v>
+      </c>
+      <c r="D1756" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1756" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F1756" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1757" t="s">
+        <v>2799</v>
+      </c>
+      <c r="B1757" t="s">
+        <v>2800</v>
+      </c>
+      <c r="C1757">
+        <v>1</v>
+      </c>
+      <c r="D1757" t="s">
+        <v>2801</v>
+      </c>
+      <c r="E1757" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1757" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1758" t="s">
+        <v>2802</v>
+      </c>
+      <c r="B1758" t="s">
+        <v>2803</v>
+      </c>
+      <c r="C1758">
+        <v>2</v>
+      </c>
+      <c r="D1758" t="s">
+        <v>2804</v>
+      </c>
+      <c r="E1758" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1758" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1759" t="s">
+        <v>2802</v>
+      </c>
+      <c r="B1759" t="s">
+        <v>2176</v>
+      </c>
+      <c r="C1759">
+        <v>5</v>
+      </c>
+      <c r="D1759" t="s">
+        <v>2177</v>
+      </c>
+      <c r="E1759" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1759" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1760" t="s">
+        <v>2802</v>
+      </c>
+      <c r="B1760" t="s">
+        <v>2805</v>
+      </c>
+      <c r="C1760">
+        <v>35</v>
+      </c>
+      <c r="D1760" t="s">
+        <v>2806</v>
+      </c>
+      <c r="E1760" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1760" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1761" t="s">
+        <v>2807</v>
+      </c>
+      <c r="B1761" t="s">
+        <v>2500</v>
+      </c>
+      <c r="C1761">
+        <v>1</v>
+      </c>
+      <c r="D1761" t="s">
+        <v>2501</v>
+      </c>
+      <c r="E1761" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1761" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1762" t="s">
+        <v>2808</v>
+      </c>
+      <c r="B1762" t="s">
+        <v>2129</v>
+      </c>
+      <c r="C1762">
+        <v>1</v>
+      </c>
+      <c r="D1762" t="s">
+        <v>2130</v>
+      </c>
+      <c r="E1762" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1762" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1763" t="s">
+        <v>2809</v>
+      </c>
+      <c r="B1763" t="s">
+        <v>2810</v>
+      </c>
+      <c r="C1763">
+        <v>2</v>
+      </c>
+      <c r="D1763" t="s">
+        <v>2811</v>
+      </c>
+      <c r="E1763" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1763" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1764" t="s">
+        <v>2812</v>
+      </c>
+      <c r="B1764" t="s">
+        <v>2813</v>
+      </c>
+      <c r="C1764">
+        <v>10</v>
+      </c>
+      <c r="D1764" t="s">
+        <v>2814</v>
+      </c>
+      <c r="E1764" t="s">
+        <v>687</v>
+      </c>
+      <c r="F1764" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1765" t="s">
+        <v>2815</v>
+      </c>
+      <c r="B1765" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1765">
+        <v>2</v>
+      </c>
+      <c r="D1765" t="s">
+        <v>268</v>
+      </c>
+      <c r="E1765" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1765" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1766" t="s">
+        <v>2815</v>
+      </c>
+      <c r="B1766" t="s">
+        <v>623</v>
+      </c>
+      <c r="C1766">
+        <v>2</v>
+      </c>
+      <c r="D1766" t="s">
+        <v>624</v>
+      </c>
+      <c r="E1766" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1766" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1767" t="s">
+        <v>2816</v>
+      </c>
+      <c r="B1767" t="s">
+        <v>2817</v>
+      </c>
+      <c r="C1767">
+        <v>2</v>
+      </c>
+      <c r="D1767" t="s">
+        <v>2818</v>
+      </c>
+      <c r="E1767" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1767" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1768" t="s">
+        <v>2816</v>
+      </c>
+      <c r="B1768" t="s">
+        <v>940</v>
+      </c>
+      <c r="C1768">
+        <v>1</v>
+      </c>
+      <c r="D1768" t="s">
+        <v>941</v>
+      </c>
+      <c r="E1768" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1768" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1769" t="s">
+        <v>2819</v>
+      </c>
+      <c r="B1769" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1769">
+        <v>1</v>
+      </c>
+      <c r="D1769" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1769" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1769" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1770" t="s">
+        <v>2820</v>
+      </c>
+      <c r="B1770" t="s">
+        <v>411</v>
+      </c>
+      <c r="C1770">
+        <v>4</v>
+      </c>
+      <c r="D1770" t="s">
+        <v>412</v>
+      </c>
+      <c r="E1770" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1770" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1771" t="s">
+        <v>2821</v>
+      </c>
+      <c r="B1771" t="s">
+        <v>323</v>
+      </c>
+      <c r="C1771">
+        <v>1</v>
+      </c>
+      <c r="D1771" t="s">
+        <v>324</v>
+      </c>
+      <c r="E1771" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1771" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1772" t="s">
+        <v>2821</v>
+      </c>
+      <c r="B1772" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1772">
+        <v>1</v>
+      </c>
+      <c r="D1772" t="s">
+        <v>287</v>
+      </c>
+      <c r="E1772" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1772" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1773" t="s">
+        <v>2822</v>
+      </c>
+      <c r="B1773" t="s">
+        <v>2823</v>
+      </c>
+      <c r="C1773">
+        <v>30</v>
+      </c>
+      <c r="D1773" t="s">
+        <v>2824</v>
+      </c>
+      <c r="E1773" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1773" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1774" t="s">
+        <v>2822</v>
+      </c>
+      <c r="B1774" t="s">
+        <v>2825</v>
+      </c>
+      <c r="C1774">
+        <v>30</v>
+      </c>
+      <c r="D1774" t="s">
+        <v>2826</v>
+      </c>
+      <c r="E1774" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1774" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1775" t="s">
+        <v>2822</v>
+      </c>
+      <c r="B1775" t="s">
+        <v>2827</v>
+      </c>
+      <c r="C1775">
+        <v>12</v>
+      </c>
+      <c r="D1775" t="s">
+        <v>2828</v>
+      </c>
+      <c r="E1775" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1775" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1776" t="s">
+        <v>2822</v>
+      </c>
+      <c r="B1776" t="s">
+        <v>1988</v>
+      </c>
+      <c r="C1776">
+        <v>12</v>
+      </c>
+      <c r="D1776" t="s">
+        <v>1989</v>
+      </c>
+      <c r="E1776" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1776" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1777" t="s">
+        <v>2829</v>
+      </c>
+      <c r="B1777" t="s">
+        <v>2830</v>
+      </c>
+      <c r="C1777">
+        <v>1</v>
+      </c>
+      <c r="D1777" t="s">
+        <v>2831</v>
+      </c>
+      <c r="E1777" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1777" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1778" t="s">
+        <v>2832</v>
+      </c>
+      <c r="B1778" t="s">
+        <v>2066</v>
+      </c>
+      <c r="C1778">
+        <v>1</v>
+      </c>
+      <c r="D1778" t="s">
+        <v>2067</v>
+      </c>
+      <c r="E1778" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1778" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1779" t="s">
+        <v>2833</v>
+      </c>
+      <c r="B1779" t="s">
+        <v>940</v>
+      </c>
+      <c r="C1779">
+        <v>5</v>
+      </c>
+      <c r="D1779" t="s">
+        <v>941</v>
+      </c>
+      <c r="E1779" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1779" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1780" t="s">
+        <v>2833</v>
+      </c>
+      <c r="B1780" t="s">
+        <v>940</v>
+      </c>
+      <c r="C1780">
+        <v>58</v>
+      </c>
+      <c r="D1780" t="s">
+        <v>941</v>
+      </c>
+      <c r="E1780" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1780" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1781" t="s">
+        <v>2834</v>
+      </c>
+      <c r="B1781" t="s">
+        <v>813</v>
+      </c>
+      <c r="C1781">
+        <v>30</v>
+      </c>
+      <c r="D1781" t="s">
+        <v>814</v>
+      </c>
+      <c r="E1781" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1781" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1782" t="s">
+        <v>2835</v>
+      </c>
+      <c r="B1782" t="s">
+        <v>2066</v>
+      </c>
+      <c r="C1782">
+        <v>1</v>
+      </c>
+      <c r="D1782" t="s">
+        <v>2067</v>
+      </c>
+      <c r="E1782" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1782" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1783" t="s">
+        <v>2836</v>
+      </c>
+      <c r="B1783" t="s">
+        <v>813</v>
+      </c>
+      <c r="C1783">
+        <v>1</v>
+      </c>
+      <c r="D1783" t="s">
+        <v>814</v>
+      </c>
+      <c r="E1783" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1783" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1784" t="s">
+        <v>2837</v>
+      </c>
+      <c r="B1784" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1784">
+        <v>2</v>
+      </c>
+      <c r="D1784" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1784" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1784" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1785" t="s">
+        <v>2838</v>
+      </c>
+      <c r="B1785" t="s">
+        <v>2839</v>
+      </c>
+      <c r="C1785">
+        <v>2</v>
+      </c>
+      <c r="D1785" t="s">
+        <v>2840</v>
+      </c>
+      <c r="E1785" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1785" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1786" t="s">
+        <v>2841</v>
+      </c>
+      <c r="B1786" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1786">
+        <v>8</v>
+      </c>
+      <c r="D1786" t="s">
+        <v>252</v>
+      </c>
+      <c r="E1786" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1786" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1787" t="s">
+        <v>2842</v>
+      </c>
+      <c r="B1787" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C1787">
+        <v>2</v>
+      </c>
+      <c r="D1787" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E1787" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1787" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1788" t="s">
+        <v>2842</v>
+      </c>
+      <c r="B1788" t="s">
+        <v>2843</v>
+      </c>
+      <c r="C1788">
+        <v>2</v>
+      </c>
+      <c r="D1788" t="s">
+        <v>1494</v>
+      </c>
+      <c r="E1788" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1788" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1789" t="s">
+        <v>2844</v>
+      </c>
+      <c r="B1789" t="s">
+        <v>308</v>
+      </c>
+      <c r="C1789">
+        <v>10</v>
+      </c>
+      <c r="D1789" t="s">
+        <v>309</v>
+      </c>
+      <c r="E1789" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1789" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1790" t="s">
+        <v>2845</v>
+      </c>
+      <c r="B1790" t="s">
+        <v>2693</v>
+      </c>
+      <c r="C1790">
+        <v>78</v>
+      </c>
+      <c r="D1790" t="s">
+        <v>2694</v>
+      </c>
+      <c r="E1790" t="s">
+        <v>389</v>
+      </c>
+      <c r="F1790" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1791" t="s">
+        <v>2846</v>
+      </c>
+      <c r="B1791" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1791">
+        <v>2</v>
+      </c>
+      <c r="D1791" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1791" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1791" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1792" t="s">
+        <v>2847</v>
+      </c>
+      <c r="B1792" t="s">
+        <v>2848</v>
+      </c>
+      <c r="C1792">
+        <v>2</v>
+      </c>
+      <c r="D1792" t="s">
+        <v>2849</v>
+      </c>
+      <c r="E1792" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1792" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1793" t="s">
+        <v>2850</v>
+      </c>
+      <c r="B1793" t="s">
+        <v>2536</v>
+      </c>
+      <c r="C1793">
+        <v>1</v>
+      </c>
+      <c r="D1793" t="s">
+        <v>2537</v>
+      </c>
+      <c r="E1793" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1793" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1794" t="s">
+        <v>2850</v>
+      </c>
+      <c r="B1794" t="s">
+        <v>2534</v>
+      </c>
+      <c r="C1794">
+        <v>1</v>
+      </c>
+      <c r="D1794" t="s">
+        <v>2535</v>
+      </c>
+      <c r="E1794" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1794" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1795" t="s">
+        <v>2851</v>
+      </c>
+      <c r="B1795" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C1795">
+        <v>3</v>
+      </c>
+      <c r="D1795" t="s">
+        <v>1728</v>
+      </c>
+      <c r="E1795" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1795" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1796" t="s">
+        <v>2852</v>
+      </c>
+      <c r="B1796" t="s">
+        <v>2853</v>
+      </c>
+      <c r="C1796">
+        <v>102</v>
+      </c>
+      <c r="D1796" t="s">
+        <v>2854</v>
+      </c>
+      <c r="E1796" t="s">
+        <v>1136</v>
+      </c>
+      <c r="F1796" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1797" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1797" t="s">
+        <v>2855</v>
+      </c>
+      <c r="B1797" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1797">
+        <v>9</v>
+      </c>
+      <c r="D1797" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1797" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1797" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1798" t="s">
+        <v>2856</v>
+      </c>
+      <c r="B1798" t="s">
+        <v>1715</v>
+      </c>
+      <c r="C1798">
+        <v>1</v>
+      </c>
+      <c r="D1798" t="s">
+        <v>1716</v>
+      </c>
+      <c r="E1798" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1798" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1799" t="s">
+        <v>2857</v>
+      </c>
+      <c r="B1799" t="s">
+        <v>458</v>
+      </c>
+      <c r="C1799">
+        <v>10</v>
+      </c>
+      <c r="D1799" t="s">
+        <v>459</v>
+      </c>
+      <c r="E1799" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1799" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1800" t="s">
+        <v>2858</v>
+      </c>
+      <c r="B1800" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C1800">
+        <v>8</v>
+      </c>
+      <c r="D1800" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E1800" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1800" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1801" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1801" t="s">
+        <v>2858</v>
+      </c>
+      <c r="B1801" t="s">
+        <v>906</v>
+      </c>
+      <c r="C1801">
+        <v>8</v>
+      </c>
+      <c r="D1801" t="s">
+        <v>907</v>
+      </c>
+      <c r="E1801" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1801" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1802" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1802" t="s">
+        <v>2859</v>
+      </c>
+      <c r="B1802" t="s">
+        <v>2860</v>
+      </c>
+      <c r="C1802">
+        <v>2</v>
+      </c>
+      <c r="D1802" t="s">
+        <v>2861</v>
+      </c>
+      <c r="E1802" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1802" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1803" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1803" t="s">
+        <v>2862</v>
+      </c>
+      <c r="B1803" t="s">
+        <v>772</v>
+      </c>
+      <c r="C1803">
+        <v>3</v>
+      </c>
+      <c r="D1803" t="s">
+        <v>773</v>
+      </c>
+      <c r="E1803" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1803" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1804" t="s">
+        <v>2862</v>
+      </c>
+      <c r="B1804" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1804">
+        <v>5</v>
+      </c>
+      <c r="D1804" t="s">
+        <v>287</v>
+      </c>
+      <c r="E1804" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1804" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1805" t="s">
+        <v>2862</v>
+      </c>
+      <c r="B1805" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C1805">
+        <v>2</v>
+      </c>
+      <c r="D1805" t="s">
+        <v>1515</v>
+      </c>
+      <c r="E1805" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1805" t="s">
+        <v>2665</v>
+      </c>
+    </row>
+    <row r="1806" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1806" t="s">
+        <v>2862</v>
+      </c>
+      <c r="B1806" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1806">
+        <v>1</v>
+      </c>
+      <c r="D1806" t="s">
+        <v>287</v>
+      </c>
+      <c r="E1806" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1806" t="s">
+        <v>2665</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>